<commit_message>
I created a concrete example of the model and some documentations about how should the proccess need to be
</commit_message>
<xml_diff>
--- a/AHP/ProcessExample.xlsx
+++ b/AHP/ProcessExample.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dados\bayswater\AFFORDABLE_HOME_LONDON\AHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7687A5FD-B92F-4D4B-ABCF-3634798B7495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6EBE5-2E31-4A83-9308-6B0A35B7141E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{466D1257-3C2C-4B7F-8506-A7EF68F8EFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="article example" sheetId="1" r:id="rId1"/>
-    <sheet name="example" sheetId="2" r:id="rId2"/>
+    <sheet name="our context example" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E60395-01E4-474E-976C-CCBDBCE99CB0}">
   <dimension ref="B2:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,39 +1179,39 @@
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>294</v>
+        <v>443</v>
       </c>
       <c r="E5">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>839</v>
+        <v>164</v>
       </c>
       <c r="F5">
         <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>9.8626269849060311E-2</v>
+        <v>0.26069482600394611</v>
       </c>
       <c r="H5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I5">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>172</v>
+        <v>480</v>
       </c>
       <c r="J5">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>751</v>
+        <v>178</v>
       </c>
       <c r="K5">
         <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -1220,39 +1220,39 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C36" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D36" ca="1" si="1">RANDBETWEEN(100,500)</f>
-        <v>406</v>
+        <v>301</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E36" ca="1" si="2">RANDBETWEEN(1,1000)</f>
-        <v>991</v>
+        <v>697</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F36" ca="1" si="3">RANDBETWEEN(1,50)</f>
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G36" ca="1" si="4">RAND()</f>
-        <v>0.57858047625821396</v>
+        <v>0.78124481137699153</v>
       </c>
       <c r="H6">
         <f t="shared" ref="H6:H36" ca="1" si="5">RANDBETWEEN(1,100)</f>
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:I36" ca="1" si="6">RANDBETWEEN(100,500)</f>
-        <v>456</v>
+        <v>326</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J36" ca="1" si="7">RANDBETWEEN(1,1000)</f>
-        <v>205</v>
+        <v>580</v>
       </c>
       <c r="K6">
         <f t="shared" ref="K6:K36" ca="1" si="8">RANDBETWEEN(1,50)</f>
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -1261,39 +1261,39 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>449</v>
+        <v>395</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>484</v>
+        <v>345</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="4"/>
-        <v>0.86473480755027554</v>
+        <v>0.83424756989159143</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="5"/>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="6"/>
-        <v>400</v>
+        <v>201</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="7"/>
-        <v>426</v>
+        <v>117</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1302,39 +1302,39 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>363</v>
+        <v>287</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>348</v>
+        <v>295</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.61750284179702208</v>
+        <v>0.70011411001172297</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="5"/>
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="6"/>
-        <v>429</v>
+        <v>201</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="7"/>
-        <v>884</v>
+        <v>274</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -1343,39 +1343,39 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>172</v>
+        <v>311</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="4"/>
-        <v>8.3193114457258077E-2</v>
+        <v>0.48452393133716165</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="5"/>
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="6"/>
-        <v>469</v>
+        <v>288</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="7"/>
-        <v>174</v>
+        <v>598</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -1384,39 +1384,39 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>365</v>
+        <v>325</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>459</v>
+        <v>873</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27758018299067588</v>
+        <v>0.66232257435370701</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="6"/>
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="7"/>
-        <v>472</v>
+        <v>752</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -1425,39 +1425,39 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>892</v>
+        <v>535</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1289515066973683E-2</v>
+        <v>0.17492483484724786</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="6"/>
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>504</v>
+        <v>32</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="8"/>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1466,39 +1466,39 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>322</v>
+        <v>475</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>460</v>
+        <v>853</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="4"/>
-        <v>0.18785834686019809</v>
+        <v>0.23191537805853291</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="6"/>
-        <v>116</v>
+        <v>273</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="7"/>
-        <v>855</v>
+        <v>652</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -1507,39 +1507,39 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>525</v>
+        <v>271</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="4"/>
-        <v>0.5667252673750226</v>
+        <v>0.72881800762123494</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="6"/>
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="7"/>
-        <v>549</v>
+        <v>744</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -1548,39 +1548,39 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="2"/>
-        <v>128</v>
+        <v>952</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="4"/>
-        <v>0.71735911024324528</v>
+        <v>0.48405616689631814</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="6"/>
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="7"/>
-        <v>705</v>
+        <v>466</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="8"/>
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -1589,39 +1589,39 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>341</v>
+        <v>428</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
-        <v>344</v>
+        <v>767</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="4"/>
-        <v>0.30742452767241979</v>
+        <v>0.40458291174593186</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="5"/>
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="6"/>
-        <v>433</v>
+        <v>463</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="7"/>
-        <v>701</v>
+        <v>372</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="8"/>
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -1630,39 +1630,39 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>360</v>
+        <v>464</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>955</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="4"/>
-        <v>0.61372113390114658</v>
+        <v>0.11536025025368679</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="5"/>
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="6"/>
-        <v>255</v>
+        <v>483</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="7"/>
-        <v>533</v>
+        <v>28</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="8"/>
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1671,39 +1671,39 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>196</v>
+        <v>355</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>923</v>
+        <v>521</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="4"/>
-        <v>0.63851009820393123</v>
+        <v>0.98411997493609116</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="5"/>
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="6"/>
-        <v>458</v>
+        <v>357</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="7"/>
-        <v>798</v>
+        <v>427</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="8"/>
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1712,39 +1712,39 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>425</v>
+        <v>484</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
-        <v>242</v>
+        <v>587</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="4"/>
-        <v>0.46420693934189294</v>
+        <v>0.53833626561366477</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="5"/>
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="6"/>
-        <v>371</v>
+        <v>172</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="7"/>
-        <v>419</v>
+        <v>666</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="8"/>
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1753,39 +1753,39 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>170</v>
+        <v>394</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
-        <v>770</v>
+        <v>976</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="4"/>
-        <v>0.66347472040666267</v>
+        <v>0.58521165618830961</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="5"/>
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="6"/>
-        <v>466</v>
+        <v>381</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="7"/>
-        <v>930</v>
+        <v>851</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="8"/>
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1794,39 +1794,39 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
-        <v>616</v>
+        <v>852</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99519425783545479</v>
+        <v>0.65863893009722863</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="5"/>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="6"/>
-        <v>354</v>
+        <v>211</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="7"/>
-        <v>202</v>
+        <v>634</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1835,39 +1835,39 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>87</v>
+        <v>270</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="4"/>
-        <v>0.29373292311877375</v>
+        <v>0.50422933616342491</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="5"/>
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="6"/>
-        <v>398</v>
+        <v>500</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="7"/>
-        <v>569</v>
+        <v>350</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="8"/>
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1876,39 +1876,39 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>454</v>
+        <v>257</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>809</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="4"/>
-        <v>0.42554683522345327</v>
+        <v>0.72110370819582725</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="6"/>
-        <v>365</v>
+        <v>285</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="7"/>
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="8"/>
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1917,39 +1917,39 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>274</v>
+        <v>393</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
-        <v>669</v>
+        <v>333</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="4"/>
-        <v>0.20030548331022657</v>
+        <v>2.6522630815053239E-2</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="5"/>
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="6"/>
-        <v>362</v>
+        <v>386</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="7"/>
-        <v>811</v>
+        <v>179</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="8"/>
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1958,39 +1958,39 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>247</v>
+        <v>107</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>152</v>
+        <v>330</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="4"/>
-        <v>0.29609965678190897</v>
+        <v>0.14138610637360283</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="5"/>
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="6"/>
-        <v>374</v>
+        <v>147</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="7"/>
-        <v>324</v>
+        <v>343</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1999,39 +1999,39 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>463</v>
+        <v>421</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>400</v>
+        <v>636</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="4"/>
-        <v>0.44418709485587715</v>
+        <v>0.38403282323303523</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="5"/>
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="6"/>
-        <v>416</v>
+        <v>352</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="7"/>
-        <v>302</v>
+        <v>161</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -2040,39 +2040,39 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>352</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>516</v>
+        <v>346</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="4"/>
-        <v>0.63535723791663434</v>
+        <v>0.32033227604975467</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="5"/>
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="6"/>
-        <v>240</v>
+        <v>383</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="7"/>
-        <v>469</v>
+        <v>610</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -2081,39 +2081,39 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>417</v>
+        <v>335</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
-        <v>429</v>
+        <v>150</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="4"/>
-        <v>0.69055864665775668</v>
+        <v>0.46281272814794672</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="5"/>
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="6"/>
-        <v>423</v>
+        <v>491</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="7"/>
-        <v>513</v>
+        <v>281</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="8"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -2122,39 +2122,39 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>407</v>
+        <v>325</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="2"/>
-        <v>391</v>
+        <v>362</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="4"/>
-        <v>0.58205396274145471</v>
+        <v>0.61349740835547006</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="6"/>
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="7"/>
-        <v>581</v>
+        <v>376</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="8"/>
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -2163,39 +2163,39 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>116</v>
+        <v>268</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
-        <v>594</v>
+        <v>27</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="4"/>
-        <v>0.93599962844287854</v>
+        <v>0.52681639478576214</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="5"/>
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="6"/>
-        <v>303</v>
+        <v>355</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="7"/>
-        <v>780</v>
+        <v>246</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="8"/>
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -2204,39 +2204,39 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>409</v>
+        <v>291</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="4"/>
-        <v>0.48402384483966521</v>
+        <v>0.99787786997074357</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="5"/>
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="6"/>
-        <v>292</v>
+        <v>252</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="7"/>
-        <v>883</v>
+        <v>841</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="8"/>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -2245,39 +2245,39 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>390</v>
+        <v>131</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="4"/>
-        <v>0.93962424987879722</v>
+        <v>6.2524247115530729E-2</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="6"/>
-        <v>147</v>
+        <v>384</v>
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="7"/>
-        <v>529</v>
+        <v>834</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="8"/>
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -2286,39 +2286,39 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
-        <v>359</v>
+        <v>194</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="2"/>
-        <v>705</v>
+        <v>379</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="4"/>
-        <v>0.39480146496523227</v>
+        <v>0.6273079387500321</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="6"/>
-        <v>482</v>
+        <v>430</v>
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="7"/>
-        <v>335</v>
+        <v>978</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
@@ -2327,39 +2327,39 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
-        <v>375</v>
+        <v>462</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="2"/>
-        <v>473</v>
+        <v>660</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="4"/>
-        <v>0.1812304488325216</v>
+        <v>0.14719800645779368</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="6"/>
-        <v>190</v>
+        <v>424</v>
       </c>
       <c r="J33">
         <f t="shared" ca="1" si="7"/>
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="8"/>
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
@@ -2368,39 +2368,39 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>297</v>
+        <v>456</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>836</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="4"/>
-        <v>5.9088091411391819E-2</v>
+        <v>0.62326628847377219</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="5"/>
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="6"/>
-        <v>415</v>
+        <v>255</v>
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="7"/>
-        <v>835</v>
+        <v>755</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
@@ -2409,39 +2409,39 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>307</v>
+        <v>208</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="2"/>
-        <v>637</v>
+        <v>178</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="4"/>
-        <v>1.776470346994985E-2</v>
+        <v>0.59773812730504028</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="5"/>
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="6"/>
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="J35">
         <f t="shared" ca="1" si="7"/>
-        <v>411</v>
+        <v>37</v>
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -2450,39 +2450,39 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>422</v>
+        <v>386</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="2"/>
-        <v>857</v>
+        <v>178</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="4"/>
-        <v>5.7666546701521049E-2</v>
+        <v>0.76419636186392526</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="5"/>
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="6"/>
-        <v>316</v>
+        <v>392</v>
       </c>
       <c r="J36">
         <f t="shared" ca="1" si="7"/>
-        <v>464</v>
+        <v>256</v>
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="8"/>
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -2529,47 +2529,47 @@
       </c>
       <c r="C39">
         <f ca="1">C5/SUM(C$5:C$36)</f>
-        <v>6.5554231227651968E-3</v>
+        <v>2.7745664739884393E-2</v>
       </c>
       <c r="D39">
         <f t="shared" ref="D39:K39" ca="1" si="9">D5/SUM(D$5:D$36)</f>
-        <v>2.8261078535037971E-2</v>
+        <v>4.1654913023037143E-2</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="9"/>
-        <v>5.6180527655015404E-2</v>
+        <v>1.0085480597749216E-2</v>
       </c>
       <c r="F39">
         <f t="array" aca="1" ref="F39" ca="1">(1/F5)/SUM(1/F$5:F$36)</f>
-        <v>3.5213445391146687E-2</v>
+        <v>2.7390956582732641E-2</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="9"/>
-        <v>6.8518907995201344E-3</v>
+        <v>1.614214001595041E-2</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="9"/>
-        <v>2.5559105431309905E-3</v>
+        <v>5.2516411378555797E-2</v>
       </c>
       <c r="I39">
         <f t="array" aca="1" ref="I39" ca="1">(1/I5)/SUM(1/I$5:I$36)</f>
-        <v>5.2066126052161037E-2</v>
+        <v>1.86238581680645E-2</v>
       </c>
       <c r="J39">
         <f t="array" aca="1" ref="J39" ca="1">(1/J5)/SUM(1/J$5:J$36)</f>
-        <v>1.7040987908024992E-2</v>
+        <v>3.1740682535092241E-2</v>
       </c>
       <c r="K39">
         <f t="array" aca="1" ref="K39" ca="1">(1/K5)/SUM(1/K$5:K$36)</f>
-        <v>1.0237326689147945E-2</v>
+        <v>8.5947425940880867E-3</v>
       </c>
       <c r="M39">
         <f ca="1">SUMPRODUCT(C39:K39,$C$77:$K$77)</f>
-        <v>2.3049736486458094E-2</v>
+        <v>2.3311974704697327E-2</v>
       </c>
       <c r="N39">
         <f ca="1">RANK(M39,$M$39:$M$70)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -2578,47 +2578,47 @@
       </c>
       <c r="C40">
         <f t="shared" ref="C40:K70" ca="1" si="10">C6/SUM(C$5:C$36)</f>
-        <v>2.3837902264600714E-3</v>
+        <v>3.7572254335260118E-2</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="10"/>
-        <v>3.9027203691242913E-2</v>
+        <v>2.8302773859896567E-2</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="10"/>
-        <v>6.6358644703361461E-2</v>
+        <v>4.2863292540434167E-2</v>
       </c>
       <c r="F40">
         <f t="array" aca="1" ref="F40" ca="1">(1/F6)/SUM(1/F$5:F$36)</f>
-        <v>1.0670741027620207E-2</v>
+        <v>2.9102891369153432E-2</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="10"/>
-        <v>4.0195885417980304E-2</v>
+        <v>4.837442815911995E-2</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1309904153354634E-2</v>
+        <v>2.4070021881838075E-2</v>
       </c>
       <c r="I40">
         <f t="array" aca="1" ref="I40" ca="1">(1/I6)/SUM(1/I$5:I$36)</f>
-        <v>1.9638977370551969E-2</v>
+        <v>2.7421631658499881E-2</v>
       </c>
       <c r="J40">
         <f t="array" aca="1" ref="J40" ca="1">(1/J6)/SUM(1/J$5:J$36)</f>
-        <v>6.2428204482569596E-2</v>
+        <v>9.7411060193903793E-3</v>
       </c>
       <c r="K40">
         <f t="array" aca="1" ref="K40" ca="1">(1/K6)/SUM(1/K$5:K$36)</f>
-        <v>3.1735712736358633E-2</v>
+        <v>7.6804082755680776E-3</v>
       </c>
       <c r="M40">
         <f t="shared" ref="M40:M70" ca="1" si="11">SUMPRODUCT(C40:K40,$C$77:$K$77)</f>
-        <v>2.9792790695962995E-2</v>
+        <v>2.2192931582242906E-2</v>
       </c>
       <c r="N40">
         <f t="shared" ref="N40:N70" ca="1" si="12">RANK(M40,$M$39:$M$70)</f>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -2627,47 +2627,47 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8140643623361142E-2</v>
+        <v>8.0924855491329474E-3</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="10"/>
-        <v>4.3160626742285879E-2</v>
+        <v>3.7141513869299481E-2</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2409267443417704E-2</v>
+        <v>2.1216407355021217E-2</v>
       </c>
       <c r="F41">
         <f t="array" aca="1" ref="F41" ca="1">(1/F7)/SUM(1/F$5:F$36)</f>
-        <v>9.0290885618324827E-3</v>
+        <v>2.0245489648106737E-2</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="10"/>
-        <v>6.0075966382449567E-2</v>
+        <v>5.1656341967264839E-2</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="10"/>
-        <v>4.984025559105431E-2</v>
+        <v>4.1575492341356671E-2</v>
       </c>
       <c r="I41">
         <f t="array" aca="1" ref="I41" ca="1">(1/I7)/SUM(1/I$5:I$36)</f>
-        <v>2.2388434202429249E-2</v>
+        <v>4.4474885177467463E-2</v>
       </c>
       <c r="J41">
         <f t="array" aca="1" ref="J41" ca="1">(1/J7)/SUM(1/J$5:J$36)</f>
-        <v>3.0041741593724809E-2</v>
+        <v>4.8289243514926666E-2</v>
       </c>
       <c r="K41">
         <f t="array" aca="1" ref="K41" ca="1">(1/K7)/SUM(1/K$5:K$36)</f>
-        <v>4.5336732480512329E-2</v>
+        <v>1.4439167558067987E-2</v>
       </c>
       <c r="M41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.3092512124722043E-2</v>
+        <v>2.8857153426484535E-2</v>
       </c>
       <c r="N41">
         <f t="shared" ca="1" si="12"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -2676,47 +2676,47 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="10"/>
-        <v>2.562574493444577E-2</v>
+        <v>5.4913294797687862E-2</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="10"/>
-        <v>3.4893780640199941E-2</v>
+        <v>2.698636577338975E-2</v>
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="10"/>
-        <v>2.3302531137002813E-2</v>
+        <v>1.8141565709365967E-2</v>
       </c>
       <c r="F42">
         <f t="array" aca="1" ref="F42" ca="1">(1/F8)/SUM(1/F$5:F$36)</f>
-        <v>5.8689075651911143E-2</v>
+        <v>1.5521542063548497E-2</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="10"/>
-        <v>4.2899949951081567E-2</v>
+        <v>4.3350841150873759E-2</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="10"/>
-        <v>6.1341853035143772E-2</v>
+        <v>1.7505470459518599E-2</v>
       </c>
       <c r="I42">
         <f t="array" aca="1" ref="I42" ca="1">(1/I8)/SUM(1/I$5:I$36)</f>
-        <v>2.0874996925341956E-2</v>
+        <v>4.4474885177467463E-2</v>
       </c>
       <c r="J42">
         <f t="array" aca="1" ref="J42" ca="1">(1/J8)/SUM(1/J$5:J$36)</f>
-        <v>1.4477128867564219E-2</v>
+        <v>2.061985945710372E-2</v>
       </c>
       <c r="K42">
         <f t="array" aca="1" ref="K42" ca="1">(1/K8)/SUM(1/K$5:K$36)</f>
-        <v>2.1157141824239088E-2</v>
+        <v>1.0938763301566658E-2</v>
       </c>
       <c r="M42">
         <f t="shared" ca="1" si="11"/>
-        <v>3.5753029644857014E-2</v>
+        <v>2.2257465423803954E-2</v>
       </c>
       <c r="N42">
         <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -2725,47 +2725,47 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="10"/>
-        <v>1.5494636471990465E-2</v>
+        <v>4.5086705202312137E-2</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3067384408343746E-2</v>
+        <v>3.2910202162670425E-2</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="10"/>
-        <v>1.1517342975760011E-2</v>
+        <v>1.9125515035975649E-2</v>
       </c>
       <c r="F43">
         <f t="array" aca="1" ref="F43" ca="1">(1/F9)/SUM(1/F$5:F$36)</f>
-        <v>0.35213445391146686</v>
+        <v>1.369547829136632E-2</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="10"/>
-        <v>5.7796988206640885E-3</v>
+        <v>3.0001566431567067E-2</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3226837060702875E-2</v>
+        <v>3.8840262582056896E-2</v>
       </c>
       <c r="I43">
         <f t="array" aca="1" ref="I43" ca="1">(1/I9)/SUM(1/I$5:I$36)</f>
-        <v>1.9094613392263749E-2</v>
+        <v>3.1039763613440834E-2</v>
       </c>
       <c r="J43">
         <f t="array" aca="1" ref="J43" ca="1">(1/J9)/SUM(1/J$5:J$36)</f>
-        <v>7.3550470798429704E-2</v>
+        <v>9.4478954703117388E-3</v>
       </c>
       <c r="K43">
         <f t="array" aca="1" ref="K43" ca="1">(1/K9)/SUM(1/K$5:K$36)</f>
-        <v>0.31735712736358634</v>
+        <v>2.2561199309481229E-2</v>
       </c>
       <c r="M43">
         <f t="shared" ca="1" si="11"/>
-        <v>0.18055972631490183</v>
+        <v>2.2099063165060127E-2</v>
       </c>
       <c r="N43">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -2774,47 +2774,47 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6686531585220502E-2</v>
+        <v>5.722543352601156E-2</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="10"/>
-        <v>3.5086032875132171E-2</v>
+        <v>3.0559473436765398E-2</v>
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0735235034150262E-2</v>
+        <v>5.3686735133140644E-2</v>
       </c>
       <c r="F44">
         <f t="array" aca="1" ref="F44" ca="1">(1/F10)/SUM(1/F$5:F$36)</f>
-        <v>1.4672268912977786E-2</v>
+        <v>1.0122744824053368E-2</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="10"/>
-        <v>1.9284406729299503E-2</v>
+        <v>4.1010801383455274E-2</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8338658146964855E-2</v>
+        <v>4.2122538293216633E-2</v>
       </c>
       <c r="I44">
         <f t="array" aca="1" ref="I44" ca="1">(1/I10)/SUM(1/I$5:I$36)</f>
-        <v>2.0306969798121768E-2</v>
+        <v>2.0741187750976706E-2</v>
       </c>
       <c r="J44">
         <f t="array" aca="1" ref="J44" ca="1">(1/J10)/SUM(1/J$5:J$36)</f>
-        <v>2.7113944743488914E-2</v>
+        <v>7.5130870894234304E-3</v>
       </c>
       <c r="K44">
         <f t="array" aca="1" ref="K44" ca="1">(1/K10)/SUM(1/K$5:K$36)</f>
-        <v>0.10578570912119543</v>
+        <v>0.36097918895169967</v>
       </c>
       <c r="M44">
         <f t="shared" ca="1" si="11"/>
-        <v>4.2338152052679032E-2</v>
+        <v>0.11097943188169634</v>
       </c>
       <c r="N44">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
@@ -2823,47 +2823,47 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="10"/>
-        <v>5.2443384982121574E-2</v>
+        <v>3.6994219653179193E-2</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="10"/>
-        <v>3.5182158992598286E-2</v>
+        <v>3.5260930888575459E-2</v>
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="10"/>
-        <v>5.9729476362662383E-2</v>
+        <v>3.2900805608511163E-2</v>
       </c>
       <c r="F45">
         <f t="array" aca="1" ref="F45" ca="1">(1/F11)/SUM(1/F$5:F$36)</f>
-        <v>7.0426890782293375E-3</v>
+        <v>1.5020847158272739E-2</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="10"/>
-        <v>5.6474495206730877E-3</v>
+        <v>1.0831289671734932E-2</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="10"/>
-        <v>4.1533546325878593E-2</v>
+        <v>5.3063457330415752E-2</v>
       </c>
       <c r="I45">
         <f t="array" aca="1" ref="I45" ca="1">(1/I11)/SUM(1/I$5:I$36)</f>
-        <v>3.7159226891998749E-2</v>
+        <v>3.9908267502995358E-2</v>
       </c>
       <c r="J45">
         <f t="array" aca="1" ref="J45" ca="1">(1/J11)/SUM(1/J$5:J$36)</f>
-        <v>2.5392424442315015E-2</v>
+        <v>0.17655754660145062</v>
       </c>
       <c r="K45">
         <f t="array" aca="1" ref="K45" ca="1">(1/K11)/SUM(1/K$5:K$36)</f>
-        <v>7.5561220800853882E-3</v>
+        <v>8.2040724761749933E-3</v>
       </c>
       <c r="M45">
         <f t="shared" ca="1" si="11"/>
-        <v>2.1876902101289099E-2</v>
+        <v>5.253157417797169E-2</v>
       </c>
       <c r="N45">
         <f t="shared" ca="1" si="12"/>
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
@@ -2872,47 +2872,47 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="10"/>
-        <v>1.0727056019070322E-2</v>
+        <v>4.797687861271676E-2</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0952609824089206E-2</v>
+        <v>4.4663845792195581E-2</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0802196330520958E-2</v>
+        <v>5.2456798474878545E-2</v>
       </c>
       <c r="F46">
         <f t="array" aca="1" ref="F46" ca="1">(1/F12)/SUM(1/F$5:F$36)</f>
-        <v>7.6550968241623227E-3</v>
+        <v>1.5521542063548497E-2</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="10"/>
-        <v>1.3051136177353029E-2</v>
+        <v>1.4360125829333666E-2</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8977635782747606E-2</v>
+        <v>1.6411378555798686E-2</v>
       </c>
       <c r="I46">
         <f t="array" aca="1" ref="I46" ca="1">(1/I12)/SUM(1/I$5:I$36)</f>
-        <v>7.7201497249756029E-2</v>
+        <v>3.2745245130662862E-2</v>
       </c>
       <c r="J46">
         <f t="array" aca="1" ref="J46" ca="1">(1/J12)/SUM(1/J$5:J$36)</f>
-        <v>1.4968165987048851E-2</v>
+        <v>8.6654010601938947E-3</v>
       </c>
       <c r="K46">
         <f t="array" aca="1" ref="K46" ca="1">(1/K12)/SUM(1/K$5:K$36)</f>
-        <v>1.6703006703346648E-2</v>
+        <v>6.0163198158616607E-2</v>
       </c>
       <c r="M46">
         <f t="shared" ca="1" si="11"/>
-        <v>2.0313740080826977E-2</v>
+        <v>3.2537649772406287E-2</v>
       </c>
       <c r="N46">
         <f t="shared" ca="1" si="12"/>
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -2921,47 +2921,47 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="10"/>
-        <v>5.6615017878426696E-2</v>
+        <v>3.236994219653179E-2</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="10"/>
-        <v>1.7494953378833028E-2</v>
+        <v>1.1847672778561354E-2</v>
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="10"/>
-        <v>3.5154680594616315E-2</v>
+        <v>1.6665641719451448E-2</v>
       </c>
       <c r="F47">
         <f t="array" aca="1" ref="F47" ca="1">(1/F13)/SUM(1/F$5:F$36)</f>
-        <v>7.0426890782293375E-2</v>
+        <v>3.5818943223573457E-2</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="10"/>
-        <v>3.9372265131038038E-2</v>
+        <v>4.5128177284922057E-2</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="10"/>
-        <v>1.2140575079872205E-2</v>
+        <v>3.2275711159737416E-2</v>
       </c>
       <c r="I47">
         <f t="array" aca="1" ref="I47" ca="1">(1/I13)/SUM(1/I$5:I$36)</f>
-        <v>5.5971085506073118E-2</v>
+        <v>4.8583977829733484E-2</v>
       </c>
       <c r="J47">
         <f t="array" aca="1" ref="J47" ca="1">(1/J13)/SUM(1/J$5:J$36)</f>
-        <v>2.3311078176551491E-2</v>
+        <v>7.5938729721054029E-3</v>
       </c>
       <c r="K47">
         <f t="array" aca="1" ref="K47" ca="1">(1/K13)/SUM(1/K$5:K$36)</f>
-        <v>2.1157141824239088E-2</v>
+        <v>6.0163198158616607E-2</v>
       </c>
       <c r="M47">
         <f t="shared" ca="1" si="11"/>
-        <v>4.0717779189760508E-2</v>
+        <v>3.4806448817439453E-2</v>
       </c>
       <c r="N47">
         <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
@@ -2970,47 +2970,47 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="10"/>
-        <v>4.8271752085816445E-2</v>
+        <v>3.8728323699421967E-2</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="10"/>
-        <v>2.2012880899740458E-2</v>
+        <v>2.3413258110014105E-2</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="10"/>
-        <v>8.5710459354493111E-3</v>
+        <v>5.8544984933275937E-2</v>
       </c>
       <c r="F48">
         <f t="array" aca="1" ref="F48" ca="1">(1/F14)/SUM(1/F$5:F$36)</f>
-        <v>1.9563025217303714E-2</v>
+        <v>1.6056767651946722E-2</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="10"/>
-        <v>4.9837292791769044E-2</v>
+        <v>2.9972602607411754E-2</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6613418530351438E-2</v>
+        <v>4.8687089715536105E-2</v>
       </c>
       <c r="I48">
         <f t="array" aca="1" ref="I48" ca="1">(1/I14)/SUM(1/I$5:I$36)</f>
-        <v>4.455409791528208E-2</v>
+        <v>3.9730897425204269E-2</v>
       </c>
       <c r="J48">
         <f t="array" aca="1" ref="J48" ca="1">(1/J14)/SUM(1/J$5:J$36)</f>
-        <v>1.8152882154506056E-2</v>
+        <v>1.2124123371773432E-2</v>
       </c>
       <c r="K48">
         <f t="array" aca="1" ref="K48" ca="1">(1/K14)/SUM(1/K$5:K$36)</f>
-        <v>6.3471425472717263E-3</v>
+        <v>1.2032639631723322E-2</v>
       </c>
       <c r="M48">
         <f t="shared" ca="1" si="11"/>
-        <v>2.1590355141052578E-2</v>
+        <v>2.3345893122306303E-2</v>
       </c>
       <c r="N48">
         <f t="shared" ca="1" si="12"/>
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
@@ -3019,47 +3019,47 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="10"/>
-        <v>5.9594755661501785E-3</v>
+        <v>1.7341040462427746E-3</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2779006055945401E-2</v>
+        <v>4.024447578749412E-2</v>
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="10"/>
-        <v>2.3034685951520022E-2</v>
+        <v>4.7168070844351519E-2</v>
       </c>
       <c r="F49">
         <f t="array" aca="1" ref="F49" ca="1">(1/F15)/SUM(1/F$5:F$36)</f>
-        <v>2.5152460993676202E-2</v>
+        <v>1.2934618386290413E-2</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="10"/>
-        <v>2.1357791346354418E-2</v>
+        <v>2.5051644137213849E-2</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="10"/>
-        <v>5.6230031948881792E-2</v>
+        <v>3.0087527352297593E-2</v>
       </c>
       <c r="I49">
         <f t="array" aca="1" ref="I49" ca="1">(1/I15)/SUM(1/I$5:I$36)</f>
-        <v>2.0682156307093993E-2</v>
+        <v>1.9307671534926484E-2</v>
       </c>
       <c r="J49">
         <f t="array" aca="1" ref="J49" ca="1">(1/J15)/SUM(1/J$5:J$36)</f>
-        <v>1.8256464934274991E-2</v>
+        <v>1.5187745944210806E-2</v>
       </c>
       <c r="K49">
         <f t="array" aca="1" ref="K49" ca="1">(1/K15)/SUM(1/K$5:K$36)</f>
-        <v>9.6168826473814039E-3</v>
+        <v>8.8043704622365777E-3</v>
       </c>
       <c r="M49">
         <f t="shared" ca="1" si="11"/>
-        <v>2.0933565041075242E-2</v>
+        <v>1.7279255421849594E-2</v>
       </c>
       <c r="N49">
         <f t="shared" ca="1" si="12"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
@@ -3068,47 +3068,47 @@
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8009535160905839E-2</v>
+        <v>4.6242774566473986E-2</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="10"/>
-        <v>3.4605402287801595E-2</v>
+        <v>4.3629525152797367E-2</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6740324092674435E-3</v>
+        <v>5.8729475432015253E-2</v>
       </c>
       <c r="F50">
         <f t="array" aca="1" ref="F50" ca="1">(1/F16)/SUM(1/F$5:F$36)</f>
-        <v>7.8252100869214865E-3</v>
+        <v>9.9073672746054237E-3</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="10"/>
-        <v>4.2637222286556913E-2</v>
+        <v>7.1430696972938921E-3</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="10"/>
-        <v>3.9616613418530351E-2</v>
+        <v>3.665207877461707E-2</v>
       </c>
       <c r="I50">
         <f t="array" aca="1" ref="I50" ca="1">(1/I16)/SUM(1/I$5:I$36)</f>
-        <v>3.511911247439882E-2</v>
+        <v>1.8508182030374663E-2</v>
       </c>
       <c r="J50">
         <f t="array" aca="1" ref="J50" ca="1">(1/J16)/SUM(1/J$5:J$36)</f>
-        <v>2.4010847877911384E-2</v>
+        <v>0.20178005325880069</v>
       </c>
       <c r="K50">
         <f t="array" aca="1" ref="K50" ca="1">(1/K16)/SUM(1/K$5:K$36)</f>
-        <v>9.0673464961024651E-3</v>
+        <v>1.336959959080369E-2</v>
       </c>
       <c r="M50">
         <f t="shared" ca="1" si="11"/>
-        <v>1.8559777895112393E-2</v>
+        <v>5.8440098920828333E-2</v>
       </c>
       <c r="N50">
         <f t="shared" ca="1" si="12"/>
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
@@ -3117,47 +3117,47 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="10"/>
-        <v>5.4231227651966626E-2</v>
+        <v>5.722543352601156E-2</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8840719023358647E-2</v>
+        <v>3.3380347907851431E-2</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="10"/>
-        <v>6.1805276550154012E-2</v>
+        <v>3.203984994772769E-2</v>
       </c>
       <c r="F51">
         <f t="array" aca="1" ref="F51" ca="1">(1/F17)/SUM(1/F$5:F$36)</f>
-        <v>7.6550968241623227E-3</v>
+        <v>2.1165739177566135E-2</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="10"/>
-        <v>4.4359393029664476E-2</v>
+        <v>6.0936393220445167E-2</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="10"/>
-        <v>2.4920127795527155E-2</v>
+        <v>4.5404814004376369E-2</v>
       </c>
       <c r="I51">
         <f t="array" aca="1" ref="I51" ca="1">(1/I17)/SUM(1/I$5:I$36)</f>
-        <v>1.9553217644043011E-2</v>
+        <v>2.5040481570506892E-2</v>
       </c>
       <c r="J51">
         <f t="array" aca="1" ref="J51" ca="1">(1/J17)/SUM(1/J$5:J$36)</f>
-        <v>1.6037320700409481E-2</v>
+        <v>1.323147890221644E-2</v>
       </c>
       <c r="K51">
         <f t="array" aca="1" ref="K51" ca="1">(1/K17)/SUM(1/K$5:K$36)</f>
-        <v>8.3515033516733238E-3</v>
+        <v>3.2816289904699973E-2</v>
       </c>
       <c r="M51">
         <f t="shared" ca="1" si="11"/>
-        <v>2.1960374774299653E-2</v>
+        <v>3.0792915839947924E-2</v>
       </c>
       <c r="N51">
         <f t="shared" ca="1" si="12"/>
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
@@ -3166,47 +3166,47 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="10"/>
-        <v>5.959475566150179E-2</v>
+        <v>3.0057803468208091E-2</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="10"/>
-        <v>4.0853599923099108E-2</v>
+        <v>4.5510108133521389E-2</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6204633721708852E-2</v>
+        <v>3.6098640919992618E-2</v>
       </c>
       <c r="F52">
         <f t="array" aca="1" ref="F52" ca="1">(1/F18)/SUM(1/F$5:F$36)</f>
-        <v>1.4672268912977786E-2</v>
+        <v>1.0347694709032332E-2</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2249980270144245E-2</v>
+        <v>3.333360891124134E-2</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="10"/>
-        <v>4.2811501597444089E-2</v>
+        <v>1.4223194748358862E-2</v>
       </c>
       <c r="I52">
         <f t="array" aca="1" ref="I52" ca="1">(1/I18)/SUM(1/I$5:I$36)</f>
-        <v>2.413847353361644E-2</v>
+        <v>5.1973557678319536E-2</v>
       </c>
       <c r="J52">
         <f t="array" aca="1" ref="J52" ca="1">(1/J18)/SUM(1/J$5:J$36)</f>
-        <v>3.0543632264741691E-2</v>
+        <v>8.4832454823519816E-3</v>
       </c>
       <c r="K52">
         <f t="array" aca="1" ref="K52" ca="1">(1/K18)/SUM(1/K$5:K$36)</f>
-        <v>6.3471425472717263E-3</v>
+        <v>8.2040724761749933E-3</v>
       </c>
       <c r="M52">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2905499419153822E-2</v>
+        <v>1.7941224191377923E-2</v>
       </c>
       <c r="N52">
         <f t="shared" ca="1" si="12"/>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -3215,47 +3215,47 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="10"/>
-        <v>5.1847437425506557E-2</v>
+        <v>9.2485549132947983E-3</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6341439969239643E-2</v>
+        <v>3.7047484720263278E-2</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="10"/>
-        <v>5.1560198205437259E-2</v>
+        <v>6.0020908923190452E-2</v>
       </c>
       <c r="F53">
         <f t="array" aca="1" ref="F53" ca="1">(1/F19)/SUM(1/F$5:F$36)</f>
-        <v>8.0030557707151569E-3</v>
+        <v>4.6564626190645497E-2</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="10"/>
-        <v>4.6093767303842924E-2</v>
+        <v>3.6236118061717636E-2</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0670926517571886E-2</v>
+        <v>4.8687089715536105E-2</v>
       </c>
       <c r="I53">
         <f t="array" aca="1" ref="I53" ca="1">(1/I19)/SUM(1/I$5:I$36)</f>
-        <v>1.9217540087922102E-2</v>
+        <v>2.3463128400711183E-2</v>
       </c>
       <c r="J53">
         <f t="array" aca="1" ref="J53" ca="1">(1/J19)/SUM(1/J$5:J$36)</f>
-        <v>1.3761055826802976E-2</v>
+        <v>6.6390616818406811E-3</v>
       </c>
       <c r="K53">
         <f t="array" aca="1" ref="K53" ca="1">(1/K19)/SUM(1/K$5:K$36)</f>
-        <v>9.3340331577525387E-3</v>
+        <v>7.6804082755680776E-3</v>
       </c>
       <c r="M53">
         <f t="shared" ca="1" si="11"/>
-        <v>2.1485784224531745E-2</v>
+        <v>2.4870435938132745E-2</v>
       </c>
       <c r="N53">
         <f t="shared" ca="1" si="12"/>
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
@@ -3264,47 +3264,47 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="10"/>
-        <v>4.9463647199046487E-2</v>
+        <v>4.5086705202312137E-2</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="10"/>
-        <v>4.354513121215034E-2</v>
+        <v>4.2125058768218149E-2</v>
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="10"/>
-        <v>4.1248158564349803E-2</v>
+        <v>5.2395301641965437E-2</v>
       </c>
       <c r="F54">
         <f t="array" aca="1" ref="F54" ca="1">(1/F20)/SUM(1/F$5:F$36)</f>
-        <v>1.0670741027620207E-2</v>
+        <v>0.15521542063548496</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="10"/>
-        <v>6.9139412749097198E-2</v>
+        <v>4.0782711312514916E-2</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="10"/>
-        <v>2.68370607028754E-2</v>
+        <v>3.8293216630196935E-3</v>
       </c>
       <c r="I54">
         <f t="array" aca="1" ref="I54" ca="1">(1/I20)/SUM(1/I$5:I$36)</f>
-        <v>2.5297665765456775E-2</v>
+        <v>4.2367070714080385E-2</v>
       </c>
       <c r="J54">
         <f t="array" aca="1" ref="J54" ca="1">(1/J20)/SUM(1/J$5:J$36)</f>
-        <v>6.3355356034290933E-2</v>
+        <v>8.9114219104833112E-3</v>
       </c>
       <c r="K54">
         <f t="array" aca="1" ref="K54" ca="1">(1/K20)/SUM(1/K$5:K$36)</f>
-        <v>3.9669640920448293E-2</v>
+        <v>1.3883814959680758E-2</v>
       </c>
       <c r="M54">
         <f t="shared" ca="1" si="11"/>
-        <v>3.6199303913381567E-2</v>
+        <v>4.7374381203207007E-2</v>
       </c>
       <c r="N54">
         <f t="shared" ca="1" si="12"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -3313,47 +3313,47 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="10"/>
-        <v>5.6019070321811679E-2</v>
+        <v>5.0289017341040465E-2</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="10"/>
-        <v>9.7087378640776691E-3</v>
+        <v>1.4104372355430184E-2</v>
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="10"/>
-        <v>5.8256327842507033E-3</v>
+        <v>1.6604144886538344E-2</v>
       </c>
       <c r="F55">
         <f t="array" aca="1" ref="F55" ca="1">(1/F21)/SUM(1/F$5:F$36)</f>
-        <v>4.4016806738933358E-2</v>
+        <v>4.233147835513227E-2</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0406590622496879E-2</v>
+        <v>3.1221718778479051E-2</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="10"/>
-        <v>4.7284345047923323E-2</v>
+        <v>6.0175054704595188E-3</v>
       </c>
       <c r="I55">
         <f t="array" aca="1" ref="I55" ca="1">(1/I21)/SUM(1/I$5:I$36)</f>
-        <v>2.2500938896913816E-2</v>
+        <v>1.7878903841341921E-2</v>
       </c>
       <c r="J55">
         <f t="array" aca="1" ref="J55" ca="1">(1/J21)/SUM(1/J$5:J$36)</f>
-        <v>2.2491708117621734E-2</v>
+        <v>1.6142404260704055E-2</v>
       </c>
       <c r="K55">
         <f t="array" aca="1" ref="K55" ca="1">(1/K21)/SUM(1/K$5:K$36)</f>
-        <v>6.3471425472717263E-3</v>
+        <v>7.8473736728630356E-3</v>
       </c>
       <c r="M55">
         <f t="shared" ca="1" si="11"/>
-        <v>2.6461166171702296E-2</v>
+        <v>2.1656895084625101E-2</v>
       </c>
       <c r="N55">
         <f t="shared" ca="1" si="12"/>
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
@@ -3362,47 +3362,47 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0393325387365912E-2</v>
+        <v>3.0635838150289016E-2</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="10"/>
-        <v>4.3641257329616455E-2</v>
+        <v>2.4165491302303714E-2</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6070711128967456E-3</v>
+        <v>4.9750937826701924E-2</v>
       </c>
       <c r="F56">
         <f t="array" aca="1" ref="F56" ca="1">(1/F22)/SUM(1/F$5:F$36)</f>
-        <v>3.5213445391146687E-2</v>
+        <v>1.0122744824053368E-2</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9564135899034723E-2</v>
+        <v>4.4650510338635936E-2</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="10"/>
-        <v>5.7507987220447284E-3</v>
+        <v>8.2056892778993428E-3</v>
       </c>
       <c r="I56">
         <f t="array" aca="1" ref="I56" ca="1">(1/I22)/SUM(1/I$5:I$36)</f>
-        <v>2.4535270358826574E-2</v>
+        <v>3.1366497967266531E-2</v>
       </c>
       <c r="J56">
         <f t="array" aca="1" ref="J56" ca="1">(1/J22)/SUM(1/J$5:J$36)</f>
-        <v>4.6201378768688697E-2</v>
+        <v>2.0323170831821655E-2</v>
       </c>
       <c r="K56">
         <f t="array" aca="1" ref="K56" ca="1">(1/K22)/SUM(1/K$5:K$36)</f>
-        <v>1.0943349219434011E-2</v>
+        <v>7.6804082755680776E-3</v>
       </c>
       <c r="M56">
         <f t="shared" ca="1" si="11"/>
-        <v>2.4629245823203791E-2</v>
+        <v>1.9578231057932178E-2</v>
       </c>
       <c r="N56">
         <f t="shared" ca="1" si="12"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -3411,47 +3411,47 @@
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="10"/>
-        <v>1.2514898688915376E-2</v>
+        <v>5.4335260115606937E-2</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="10"/>
-        <v>2.6338556185715657E-2</v>
+        <v>3.6953455571227083E-2</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="10"/>
-        <v>4.4797107271996789E-2</v>
+        <v>2.0478445360063956E-2</v>
       </c>
       <c r="F57">
         <f t="array" aca="1" ref="F57" ca="1">(1/F23)/SUM(1/F$5:F$36)</f>
-        <v>2.7087265685497453E-2</v>
+        <v>1.7909471611786729E-2</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="10"/>
-        <v>1.3915879615920116E-2</v>
+        <v>1.6422727937127136E-3</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="10"/>
-        <v>1.34185303514377E-2</v>
+        <v>4.7592997811816196E-2</v>
       </c>
       <c r="I57">
         <f t="array" aca="1" ref="I57" ca="1">(1/I23)/SUM(1/I$5:I$36)</f>
-        <v>2.4738601328651102E-2</v>
+        <v>2.3159201867023214E-2</v>
       </c>
       <c r="J57">
         <f t="array" aca="1" ref="J57" ca="1">(1/J23)/SUM(1/J$5:J$36)</f>
-        <v>1.5780248975248788E-2</v>
+        <v>3.1563360286292849E-2</v>
       </c>
       <c r="K57">
         <f t="array" aca="1" ref="K57" ca="1">(1/K23)/SUM(1/K$5:K$36)</f>
-        <v>1.5867856368179317E-2</v>
+        <v>2.7767629919361516E-2</v>
       </c>
       <c r="M57">
         <f t="shared" ca="1" si="11"/>
-        <v>2.1386100522394029E-2</v>
+        <v>2.7850354804822237E-2</v>
       </c>
       <c r="N57">
         <f t="shared" ca="1" si="12"/>
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -3460,47 +3460,47 @@
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="10"/>
-        <v>7.7473182359952325E-3</v>
+        <v>2.7745664739884393E-2</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="10"/>
-        <v>2.3743151014130538E-2</v>
+        <v>1.006111894687353E-2</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="10"/>
-        <v>1.0178117048346057E-2</v>
+        <v>2.0293954861324643E-2</v>
       </c>
       <c r="F58">
         <f t="array" aca="1" ref="F58" ca="1">(1/F24)/SUM(1/F$5:F$36)</f>
-        <v>1.4672268912977786E-2</v>
+        <v>3.5818943223573457E-2</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0571015381094855E-2</v>
+        <v>8.7545823612096129E-3</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7476038338658148E-2</v>
+        <v>5.3610503282275714E-2</v>
       </c>
       <c r="I58">
         <f t="array" aca="1" ref="I58" ca="1">(1/I24)/SUM(1/I$5:I$36)</f>
-        <v>2.3944849414362829E-2</v>
+        <v>6.0812598099802453E-2</v>
       </c>
       <c r="J58">
         <f t="array" aca="1" ref="J58" ca="1">(1/J24)/SUM(1/J$5:J$36)</f>
-        <v>3.94993269102678E-2</v>
+        <v>1.6471841082351078E-2</v>
       </c>
       <c r="K58">
         <f t="array" aca="1" ref="K58" ca="1">(1/K24)/SUM(1/K$5:K$36)</f>
-        <v>1.4425323971072105E-2</v>
+        <v>8.394864859341853E-3</v>
       </c>
       <c r="M58">
         <f t="shared" ca="1" si="11"/>
-        <v>1.8294764641452011E-2</v>
+        <v>2.2799206460448466E-2</v>
       </c>
       <c r="N58">
         <f t="shared" ca="1" si="12"/>
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
@@ -3509,47 +3509,47 @@
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="10"/>
-        <v>2.9797377830750892E-3</v>
+        <v>3.4104046242774563E-2</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="10"/>
-        <v>4.4506392386811498E-2</v>
+        <v>3.9586271744240717E-2</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="10"/>
-        <v>2.6784518548279096E-2</v>
+        <v>3.9111985732734764E-2</v>
       </c>
       <c r="F59">
         <f t="array" aca="1" ref="F59" ca="1">(1/F25)/SUM(1/F$5:F$36)</f>
-        <v>7.0426890782293375E-2</v>
+        <v>2.5869236772580826E-2</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="10"/>
-        <v>3.0859135939810257E-2</v>
+        <v>2.3779189247333025E-2</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="10"/>
-        <v>5.3674121405750799E-2</v>
+        <v>1.9146608315098467E-2</v>
       </c>
       <c r="I59">
         <f t="array" aca="1" ref="I59" ca="1">(1/I25)/SUM(1/I$5:I$36)</f>
-        <v>2.1527340579258893E-2</v>
+        <v>2.5396170229178866E-2</v>
       </c>
       <c r="J59">
         <f t="array" aca="1" ref="J59" ca="1">(1/J25)/SUM(1/J$5:J$36)</f>
-        <v>4.2376761320949564E-2</v>
+        <v>3.5092183175443596E-2</v>
       </c>
       <c r="K59">
         <f t="array" aca="1" ref="K59" ca="1">(1/K25)/SUM(1/K$5:K$36)</f>
-        <v>3.1735712736358633E-2</v>
+        <v>1.8998904681668403E-2</v>
       </c>
       <c r="M59">
         <f t="shared" ca="1" si="11"/>
-        <v>4.1270423396480557E-2</v>
+        <v>2.7470438120115379E-2</v>
       </c>
       <c r="N59">
         <f t="shared" ca="1" si="12"/>
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -3558,47 +3558,47 @@
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="10"/>
-        <v>3.5756853396901073E-2</v>
+        <v>3.6416184971098269E-2</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="10"/>
-        <v>9.6126117466115539E-3</v>
+        <v>3.309826046074283E-2</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="10"/>
-        <v>3.4552028927280029E-2</v>
+        <v>2.1277904187934321E-2</v>
       </c>
       <c r="F60">
         <f t="array" aca="1" ref="F60" ca="1">(1/F26)/SUM(1/F$5:F$36)</f>
-        <v>8.1891733467782998E-3</v>
+        <v>1.2585034105579863E-2</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="10"/>
-        <v>4.414035347328904E-2</v>
+        <v>1.9834871795825163E-2</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="10"/>
-        <v>3.386581469648562E-2</v>
+        <v>1.2035010940919038E-2</v>
       </c>
       <c r="I60">
         <f t="array" aca="1" ref="I60" ca="1">(1/I26)/SUM(1/I$5:I$36)</f>
-        <v>3.7314057004048745E-2</v>
+        <v>2.3340605536999896E-2</v>
       </c>
       <c r="J60">
         <f t="array" aca="1" ref="J60" ca="1">(1/J26)/SUM(1/J$5:J$36)</f>
-        <v>2.7287381490248973E-2</v>
+        <v>9.2620352315515072E-3</v>
       </c>
       <c r="K60">
         <f t="array" aca="1" ref="K60" ca="1">(1/K26)/SUM(1/K$5:K$36)</f>
-        <v>1.4425323971072105E-2</v>
+        <v>8.394864859341853E-3</v>
       </c>
       <c r="M60">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2233954520859679E-2</v>
+        <v>1.5022734236216024E-2</v>
       </c>
       <c r="N60">
         <f t="shared" ca="1" si="12"/>
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -3607,47 +3607,47 @@
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="10"/>
-        <v>5.1251489868891539E-2</v>
+        <v>5.7803468208092483E-3</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="10"/>
-        <v>4.008459098337018E-2</v>
+        <v>3.1499764927127409E-2</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8726396143029329E-2</v>
+        <v>9.2245249369657459E-3</v>
       </c>
       <c r="F61">
         <f t="array" aca="1" ref="F61" ca="1">(1/F27)/SUM(1/F$5:F$36)</f>
-        <v>7.4922224236482309E-3</v>
+        <v>1.8625850476258199E-2</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="10"/>
-        <v>4.7975376588861633E-2</v>
+        <v>2.8657215693322066E-2</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="10"/>
-        <v>2.5559105431309903E-2</v>
+        <v>5.1422319474835887E-2</v>
       </c>
       <c r="I61">
         <f t="array" aca="1" ref="I61" ca="1">(1/I27)/SUM(1/I$5:I$36)</f>
-        <v>2.1171096172509927E-2</v>
+        <v>1.8206623056356334E-2</v>
       </c>
       <c r="J61">
         <f t="array" aca="1" ref="J61" ca="1">(1/J27)/SUM(1/J$5:J$36)</f>
-        <v>2.4946943311748085E-2</v>
+        <v>2.0106197477745263E-2</v>
       </c>
       <c r="K61">
         <f t="array" aca="1" ref="K61" ca="1">(1/K27)/SUM(1/K$5:K$36)</f>
-        <v>2.2668366240256164E-2</v>
+        <v>1.164448996618386E-2</v>
       </c>
       <c r="M61">
         <f t="shared" ca="1" si="11"/>
-        <v>2.4697948163732726E-2</v>
+        <v>1.8822752693497272E-2</v>
       </c>
       <c r="N61">
         <f t="shared" ca="1" si="12"/>
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -3656,47 +3656,47 @@
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="10"/>
-        <v>4.4100119189511323E-2</v>
+        <v>2.3121387283236993E-2</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="10"/>
-        <v>3.9123329808709029E-2</v>
+        <v>3.0559473436765398E-2</v>
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="10"/>
-        <v>2.6181866880942817E-2</v>
+        <v>2.2261853514543999E-2</v>
       </c>
       <c r="F62">
         <f t="array" aca="1" ref="F62" ca="1">(1/F28)/SUM(1/F$5:F$36)</f>
-        <v>8.0030557707151569E-3</v>
+        <v>0.23282313095322746</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="10"/>
-        <v>4.0437199928943748E-2</v>
+        <v>3.7987562764083396E-2</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8530351437699679E-2</v>
+        <v>4.2122538293216633E-2</v>
       </c>
       <c r="I62">
         <f t="array" aca="1" ref="I62" ca="1">(1/I28)/SUM(1/I$5:I$36)</f>
-        <v>4.2242328683828767E-2</v>
+        <v>5.6939184208095295E-2</v>
       </c>
       <c r="J62">
         <f t="array" aca="1" ref="J62" ca="1">(1/J28)/SUM(1/J$5:J$36)</f>
-        <v>2.2027163371646761E-2</v>
+        <v>1.5026174178846861E-2</v>
       </c>
       <c r="K62">
         <f t="array" aca="1" ref="K62" ca="1">(1/K28)/SUM(1/K$5:K$36)</f>
-        <v>1.5867856368179317E-2</v>
+        <v>2.4065279263446645E-2</v>
       </c>
       <c r="M62">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2280358845357017E-2</v>
+        <v>6.413730757866036E-2</v>
       </c>
       <c r="N62">
         <f t="shared" ca="1" si="12"/>
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -3705,47 +3705,47 @@
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="10"/>
-        <v>5.2443384982121574E-2</v>
+        <v>1.2716763005780347E-2</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="10"/>
-        <v>1.1150629626069403E-2</v>
+        <v>2.5199811941701927E-2</v>
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="10"/>
-        <v>3.9775010044194453E-2</v>
+        <v>1.6604144886538342E-3</v>
       </c>
       <c r="F63">
         <f t="array" aca="1" ref="F63" ca="1">(1/F29)/SUM(1/F$5:F$36)</f>
-        <v>7.0426890782293375E-3</v>
+        <v>1.7909471611786729E-2</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="10"/>
-        <v>6.5026967483381187E-2</v>
+        <v>3.2620302204238061E-2</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7476038338658148E-2</v>
+        <v>1.3129102844638949E-2</v>
       </c>
       <c r="I63">
         <f t="array" aca="1" ref="I63" ca="1">(1/I29)/SUM(1/I$5:I$36)</f>
-        <v>2.9555688716078214E-2</v>
+        <v>2.5181554706115383E-2</v>
       </c>
       <c r="J63">
         <f t="array" aca="1" ref="J63" ca="1">(1/J29)/SUM(1/J$5:J$36)</f>
-        <v>1.640741271657278E-2</v>
+        <v>2.296683533027E-2</v>
       </c>
       <c r="K63">
         <f t="array" aca="1" ref="K63" ca="1">(1/K29)/SUM(1/K$5:K$36)</f>
-        <v>9.6168826473814039E-3</v>
+        <v>4.5122398618962459E-2</v>
       </c>
       <c r="M63">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2411763243563688E-2</v>
+        <v>2.5656239672944295E-2</v>
       </c>
       <c r="N63">
         <f t="shared" ca="1" si="12"/>
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
@@ -3754,47 +3754,47 @@
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="10"/>
-        <v>2.4433849821215731E-2</v>
+        <v>1.0982658959537572E-2</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="10"/>
-        <v>3.9315582043641259E-2</v>
+        <v>2.7362482369534556E-2</v>
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8435784116780503E-2</v>
+        <v>3.5729659922513993E-2</v>
       </c>
       <c r="F64">
         <f t="array" aca="1" ref="F64" ca="1">(1/F30)/SUM(1/F$5:F$36)</f>
-        <v>1.7606722695573344E-2</v>
+        <v>1.6630223639516245E-2</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="10"/>
-        <v>3.3626725762627652E-2</v>
+        <v>6.1788277668549808E-2</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="10"/>
-        <v>4.5367412140575082E-2</v>
+        <v>3.1728665207877461E-2</v>
       </c>
       <c r="I64">
         <f t="array" aca="1" ref="I64" ca="1">(1/I30)/SUM(1/I$5:I$36)</f>
-        <v>3.0669087948533215E-2</v>
+        <v>3.5474015558218094E-2</v>
       </c>
       <c r="J64">
         <f t="array" aca="1" ref="J64" ca="1">(1/J30)/SUM(1/J$5:J$36)</f>
-        <v>1.4493524256995209E-2</v>
+        <v>6.7180041513037088E-3</v>
       </c>
       <c r="K64">
         <f t="array" aca="1" ref="K64" ca="1">(1/K30)/SUM(1/K$5:K$36)</f>
-        <v>7.5561220800853882E-3</v>
+        <v>9.0244797237924931E-3</v>
       </c>
       <c r="M64">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2002734725986614E-2</v>
+        <v>1.8950870203107071E-2</v>
       </c>
       <c r="N64">
         <f t="shared" ca="1" si="12"/>
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
@@ -3803,47 +3803,47 @@
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="10"/>
-        <v>1.4898688915375448E-2</v>
+        <v>5.4335260115606937E-2</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="10"/>
-        <v>3.7489185811785064E-2</v>
+        <v>1.231781852374236E-2</v>
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="10"/>
-        <v>1.3860988348734431E-2</v>
+        <v>1.4267265235840354E-2</v>
       </c>
       <c r="F65">
         <f t="array" aca="1" ref="F65" ca="1">(1/F31)/SUM(1/F$5:F$36)</f>
-        <v>8.1891733467782998E-3</v>
+        <v>2.3282313095322749E-2</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="10"/>
-        <v>6.5278781835749214E-2</v>
+        <v>3.8714813285765149E-3</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1948881789137379E-3</v>
+        <v>1.8599562363238512E-2</v>
       </c>
       <c r="I65">
         <f t="array" aca="1" ref="I65" ca="1">(1/I31)/SUM(1/I$5:I$36)</f>
-        <v>6.0920909394365293E-2</v>
+        <v>2.3279822710080625E-2</v>
       </c>
       <c r="J65">
         <f t="array" aca="1" ref="J65" ca="1">(1/J31)/SUM(1/J$5:J$36)</f>
-        <v>2.4192404383604475E-2</v>
+        <v>6.7743902772738843E-3</v>
       </c>
       <c r="K65">
         <f t="array" aca="1" ref="K65" ca="1">(1/K31)/SUM(1/K$5:K$36)</f>
-        <v>9.6168826473814039E-3</v>
+        <v>5.156845556452852E-2</v>
       </c>
       <c r="M65">
         <f t="shared" ca="1" si="11"/>
-        <v>1.9768468535547173E-2</v>
+        <v>2.6788228291770133E-2</v>
       </c>
       <c r="N65">
         <f t="shared" ca="1" si="12"/>
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
@@ -3852,47 +3852,47 @@
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="10"/>
-        <v>2.6817640047675805E-2</v>
+        <v>5.7803468208092489E-4</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="10"/>
-        <v>3.450927617033548E-2</v>
+        <v>1.8241654913023039E-2</v>
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="10"/>
-        <v>4.7207713941341906E-2</v>
+        <v>2.3307299674066785E-2</v>
       </c>
       <c r="F66">
         <f t="array" aca="1" ref="F66" ca="1">(1/F32)/SUM(1/F$5:F$36)</f>
-        <v>3.5213445391146687E-2</v>
+        <v>3.8803855158871241E-2</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7428154076721573E-2</v>
+        <v>3.8842706376792401E-2</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8977635782747606E-2</v>
+        <v>1.3129102844638949E-2</v>
       </c>
       <c r="I66">
         <f t="array" aca="1" ref="I66" ca="1">(1/I32)/SUM(1/I$5:I$36)</f>
-        <v>1.8579613445999375E-2</v>
+        <v>2.0789423071327817E-2</v>
       </c>
       <c r="J66">
         <f t="array" aca="1" ref="J66" ca="1">(1/J32)/SUM(1/J$5:J$36)</f>
-        <v>3.8202334086348558E-2</v>
+        <v>5.7769340401292637E-3</v>
       </c>
       <c r="K66">
         <f t="array" aca="1" ref="K66" ca="1">(1/K32)/SUM(1/K$5:K$36)</f>
-        <v>3.526190304039848E-2</v>
+        <v>9.0244797237924931E-3</v>
       </c>
       <c r="M66">
         <f t="shared" ca="1" si="11"/>
-        <v>3.4354600484038225E-2</v>
+        <v>1.7389146213021071E-2</v>
       </c>
       <c r="N66">
         <f t="shared" ca="1" si="12"/>
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
@@ -3901,47 +3901,47 @@
       </c>
       <c r="C67">
         <f t="shared" ca="1" si="10"/>
-        <v>1.4302741358760428E-2</v>
+        <v>3.6416184971098269E-2</v>
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="10"/>
-        <v>3.604729404979333E-2</v>
+        <v>4.3441466854724962E-2</v>
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1672693183340032E-2</v>
+        <v>4.0587909722649286E-2</v>
       </c>
       <c r="F67">
         <f t="array" aca="1" ref="F67" ca="1">(1/F33)/SUM(1/F$5:F$36)</f>
-        <v>9.2666961555649165E-3</v>
+        <v>2.0245489648106737E-2</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="10"/>
-        <v>1.259067433908726E-2</v>
+        <v>9.1144533504263405E-3</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="10"/>
-        <v>6.3897763578274758E-3</v>
+        <v>3.5557986870897153E-2</v>
       </c>
       <c r="I67">
         <f t="array" aca="1" ref="I67" ca="1">(1/I33)/SUM(1/I$5:I$36)</f>
-        <v>4.7133545689324728E-2</v>
+        <v>2.1083613020450379E-2</v>
       </c>
       <c r="J67">
         <f t="array" aca="1" ref="J67" ca="1">(1/J33)/SUM(1/J$5:J$36)</f>
-        <v>0.11960543849464268</v>
+        <v>2.4999298633833714E-2</v>
       </c>
       <c r="K67">
         <f t="array" aca="1" ref="K67" ca="1">(1/K33)/SUM(1/K$5:K$36)</f>
-        <v>9.0673464961024651E-3</v>
+        <v>1.5694747345726071E-2</v>
       </c>
       <c r="M67">
         <f t="shared" ca="1" si="11"/>
-        <v>2.5059966846471222E-2</v>
+        <v>2.390081661713565E-2</v>
       </c>
       <c r="N67">
         <f t="shared" ca="1" si="12"/>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
@@ -3950,47 +3950,47 @@
       </c>
       <c r="C68">
         <f t="shared" ca="1" si="10"/>
-        <v>1.1918951132300357E-2</v>
+        <v>2.7167630057803469E-2</v>
       </c>
       <c r="D68">
         <f t="shared" ref="D68:K70" ca="1" si="13">D34/SUM(D$5:D$36)</f>
-        <v>2.8549456887436316E-2</v>
+        <v>4.2877291960507755E-2</v>
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="13"/>
-        <v>6.6961296370697743E-5</v>
+        <v>5.1411352315355756E-2</v>
       </c>
       <c r="F68">
         <f t="array" aca="1" ref="F68" ca="1">(1/F34)/SUM(1/F$5:F$36)</f>
-        <v>2.5152460993676202E-2</v>
+        <v>1.1939647741191151E-2</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="13"/>
-        <v>4.1050437223524149E-3</v>
+        <v>3.8592448687927092E-2</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="13"/>
-        <v>2.1086261980830672E-2</v>
+        <v>2.3522975929978117E-2</v>
       </c>
       <c r="I68">
         <f t="array" aca="1" ref="I68" ca="1">(1/I34)/SUM(1/I$5:I$36)</f>
-        <v>2.1579213689088432E-2</v>
+        <v>3.5056674198709649E-2</v>
       </c>
       <c r="J68">
         <f t="array" aca="1" ref="J68" ca="1">(1/J34)/SUM(1/J$5:J$36)</f>
-        <v>1.5326684932846429E-2</v>
+        <v>7.483233763240291E-3</v>
       </c>
       <c r="K68">
         <f t="array" aca="1" ref="K68" ca="1">(1/K34)/SUM(1/K$5:K$36)</f>
-        <v>0.10578570912119543</v>
+        <v>7.2195837790339945E-2</v>
       </c>
       <c r="M68">
         <f t="shared" ca="1" si="11"/>
-        <v>3.8521778257456563E-2</v>
+        <v>3.5215532679381184E-2</v>
       </c>
       <c r="N68">
         <f t="shared" ca="1" si="12"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
@@ -3999,47 +3999,47 @@
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="10"/>
-        <v>5.4231227651966626E-2</v>
+        <v>1.8497109826589597E-2</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="13"/>
-        <v>2.9510718062097471E-2</v>
+        <v>1.9558062999529856E-2</v>
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="13"/>
-        <v>4.2654345788134457E-2</v>
+        <v>1.0946436258532685E-2</v>
       </c>
       <c r="F69">
         <f t="array" aca="1" ref="F69" ca="1">(1/F35)/SUM(1/F$5:F$36)</f>
-        <v>1.4085378156458675E-2</v>
+        <v>1.0347694709032332E-2</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="13"/>
-        <v>1.2341722793352964E-3</v>
+        <v>3.7011753135767642E-2</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="13"/>
-        <v>2.7476038338658148E-2</v>
+        <v>4.7045951859956234E-2</v>
       </c>
       <c r="I69">
         <f t="array" aca="1" ref="I69" ca="1">(1/I35)/SUM(1/I$5:I$36)</f>
-        <v>3.1983477432041781E-2</v>
+        <v>3.0825696278175725E-2</v>
       </c>
       <c r="J69">
         <f t="array" aca="1" ref="J69" ca="1">(1/J35)/SUM(1/J$5:J$36)</f>
-        <v>3.1138155520503086E-2</v>
+        <v>0.15269841868233566</v>
       </c>
       <c r="K69">
         <f t="array" aca="1" ref="K69" ca="1">(1/K35)/SUM(1/K$5:K$36)</f>
-        <v>1.6703006703346648E-2</v>
+        <v>9.4994523408342014E-3</v>
       </c>
       <c r="M69">
         <f t="shared" ca="1" si="11"/>
-        <v>2.3339362274134221E-2</v>
+        <v>4.4597979103260722E-2</v>
       </c>
       <c r="N69">
         <f t="shared" ca="1" si="12"/>
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
@@ -4048,47 +4048,47 @@
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8140643623361142E-2</v>
+        <v>5.7803468208092489E-4</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="13"/>
-        <v>4.0565221570700756E-2</v>
+        <v>3.6295251527973672E-2</v>
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="13"/>
-        <v>5.7385830989687962E-2</v>
+        <v>1.0946436258532685E-2</v>
       </c>
       <c r="F70">
         <f t="array" aca="1" ref="F70" ca="1">(1/F36)/SUM(1/F$5:F$36)</f>
-        <v>9.2666961555649165E-3</v>
+        <v>1.0122744824053368E-2</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="13"/>
-        <v>4.0062843438057379E-3</v>
+        <v>4.7318793633060692E-2</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="13"/>
-        <v>5.7507987220447282E-2</v>
+        <v>3.1181619256017507E-2</v>
       </c>
       <c r="I70">
         <f t="array" aca="1" ref="I70" ca="1">(1/I36)/SUM(1/I$5:I$36)</f>
-        <v>2.8339790129657275E-2</v>
+        <v>2.2804724287425918E-2</v>
       </c>
       <c r="J70">
         <f t="array" aca="1" ref="J70" ca="1">(1/J36)/SUM(1/J$5:J$36)</f>
-        <v>2.7581426549411137E-2</v>
+        <v>2.2069693325181328E-2</v>
       </c>
       <c r="K70">
         <f t="array" aca="1" ref="K70" ca="1">(1/K36)/SUM(1/K$5:K$36)</f>
-        <v>8.3515033516733238E-3</v>
+        <v>2.2561199309481229E-2</v>
       </c>
       <c r="M70">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2158334447555609E-2</v>
+        <v>2.0545369593610439E-2</v>
       </c>
       <c r="N70">
         <f t="shared" ca="1" si="12"/>
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
@@ -4097,19 +4097,19 @@
       </c>
       <c r="C73">
         <f ca="1">AVERAGE(C39:C70)</f>
-        <v>3.1250000000000007E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="D73">
         <f t="shared" ref="D73:K73" ca="1" si="14">AVERAGE(D39:D70)</f>
-        <v>3.125E-2</v>
+        <v>3.1249999999999997E-2</v>
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="14"/>
-        <v>3.125E-2</v>
+        <v>3.1249999999999997E-2</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="14"/>
-        <v>3.1249999999999997E-2</v>
+        <v>3.1249999999999993E-2</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="14"/>
@@ -4121,15 +4121,15 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="14"/>
-        <v>3.124999999999999E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="J73">
         <f t="shared" ca="1" si="14"/>
-        <v>3.1249999999999997E-2</v>
+        <v>3.1250000000000007E-2</v>
       </c>
       <c r="K73">
         <f t="shared" ca="1" si="14"/>
-        <v>3.1250000000000007E-2</v>
+        <v>3.124999999999999E-2</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
@@ -4138,39 +4138,39 @@
       </c>
       <c r="C74">
         <f ca="1">STDEVA(C39:C70)</f>
-        <v>1.9214520703766832E-2</v>
+        <v>1.7838557348497357E-2</v>
       </c>
       <c r="D74">
         <f t="shared" ref="D74:K74" ca="1" si="15">STDEVA(D39:D70)</f>
-        <v>1.0296554844394916E-2</v>
+        <v>1.0357056338727204E-2</v>
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="15"/>
-        <v>1.8791239959628121E-2</v>
+        <v>1.7328595876783936E-2</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="15"/>
-        <v>6.1272355359712073E-2</v>
+        <v>4.4959642822510276E-2</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="15"/>
-        <v>1.96756083383391E-2</v>
+        <v>1.6140500426753402E-2</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="15"/>
-        <v>1.6253855920772477E-2</v>
+        <v>1.5733113487241442E-2</v>
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="15"/>
-        <v>1.439162005776063E-2</v>
+        <v>1.2052610769604816E-2</v>
       </c>
       <c r="J74">
         <f t="shared" ca="1" si="15"/>
-        <v>2.2093494016873504E-2</v>
+        <v>4.9038820785169912E-2</v>
       </c>
       <c r="K74">
         <f t="shared" ca="1" si="15"/>
-        <v>5.7571427870853266E-2</v>
+        <v>6.2772966765742483E-2</v>
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
@@ -4179,39 +4179,39 @@
       </c>
       <c r="C75">
         <f ca="1">C74/C73</f>
-        <v>0.61486466252053851</v>
+        <v>0.57083383515191544</v>
       </c>
       <c r="D75">
         <f t="shared" ref="D75:K75" ca="1" si="16">D74/D73</f>
-        <v>0.32948975502063732</v>
+        <v>0.33142580283927059</v>
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="16"/>
-        <v>0.60131967870809988</v>
+        <v>0.55451506805708606</v>
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="16"/>
-        <v>1.9607153715107866</v>
+        <v>1.4387085703203291</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="16"/>
-        <v>0.6296194668268511</v>
+        <v>0.51649601365610875</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="16"/>
-        <v>0.52012338946471925</v>
+        <v>0.50345963159172613</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="16"/>
-        <v>0.46053184184834034</v>
+        <v>0.3856835446273541</v>
       </c>
       <c r="J75">
         <f t="shared" ca="1" si="16"/>
-        <v>0.70699180853995225</v>
+        <v>1.5692422651254367</v>
       </c>
       <c r="K75">
         <f t="shared" ca="1" si="16"/>
-        <v>1.8422856918673041</v>
+        <v>2.0087349365037603</v>
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
@@ -4220,39 +4220,39 @@
       </c>
       <c r="C77">
         <f ca="1">C75/SUM($C$75:$K$75)</f>
-        <v>8.0207323416371074E-2</v>
+        <v>7.244911972360106E-2</v>
       </c>
       <c r="D77">
         <f t="shared" ref="D77:K77" ca="1" si="17">D75/SUM($C$75:$K$75)</f>
-        <v>4.2980989076500012E-2</v>
+        <v>4.2063918062955674E-2</v>
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="17"/>
-        <v>7.8440419309603535E-2</v>
+        <v>7.037797355427805E-2</v>
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="17"/>
-        <v>0.25576967016699009</v>
+        <v>0.18259809254433731</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="17"/>
-        <v>8.2132045120315397E-2</v>
+        <v>6.5552669140881689E-2</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="17"/>
-        <v>6.7848597355068138E-2</v>
+        <v>6.3898116893302132E-2</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="17"/>
-        <v>6.0075051689009749E-2</v>
+        <v>4.8950205084976647E-2</v>
       </c>
       <c r="J77">
         <f t="shared" ca="1" si="17"/>
-        <v>9.2225044138708953E-2</v>
+        <v>0.19916517511816978</v>
       </c>
       <c r="K77">
         <f t="shared" ca="1" si="17"/>
-        <v>0.24032085972743306</v>
+        <v>0.25494472987749767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model running with sample data, but something still unflexible yet
</commit_message>
<xml_diff>
--- a/AHP/ProcessExample.xlsx
+++ b/AHP/ProcessExample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dados\bayswater\AFFORDABLE_HOME_LONDON\AHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6EBE5-2E31-4A83-9308-6B0A35B7141E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0FCF85-2BDF-4BCE-88AE-19296B2F434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{466D1257-3C2C-4B7F-8506-A7EF68F8EFC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{466D1257-3C2C-4B7F-8506-A7EF68F8EFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="article example" sheetId="1" r:id="rId1"/>
     <sheet name="our context example" sheetId="2" r:id="rId2"/>
+    <sheet name="datamodel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -239,6 +240,24 @@
   </si>
   <si>
     <t>RANKING Order</t>
+  </si>
+  <si>
+    <t>Borough</t>
+  </si>
+  <si>
+    <t>Rent price average</t>
+  </si>
+  <si>
+    <t>Quality of life</t>
+  </si>
+  <si>
+    <t>Geo code (lat,lon)</t>
+  </si>
+  <si>
+    <t>Time to referece Borough</t>
+  </si>
+  <si>
+    <t>Runtime Calculated</t>
   </si>
 </sst>
 </file>
@@ -247,9 +266,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -322,12 +341,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,6 +356,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,7 +792,7 @@
         <v>0.44776119402985076</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6:M13" si="5">AVERAGE($H6:$J6)</f>
+        <f t="shared" ref="K6:K13" si="5">AVERAGE($H6:$J6)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="L6" s="4">
@@ -1087,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E60395-01E4-474E-976C-CCBDBCE99CB0}">
   <dimension ref="B2:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1119,7 @@
     <col min="14" max="14" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>64</v>
       </c>
@@ -1112,7 +1132,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
@@ -1141,7 +1161,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1173,496 +1193,392 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C5">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>443</v>
+        <v>331</v>
       </c>
       <c r="E5">
-        <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>164</v>
+        <v>890</v>
       </c>
       <c r="F5">
-        <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G5">
-        <f ca="1">RAND()</f>
-        <v>0.26069482600394611</v>
+        <v>6.2551379188111267E-2</v>
       </c>
       <c r="H5">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I5">
-        <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>480</v>
+        <v>162</v>
       </c>
       <c r="J5">
-        <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>178</v>
+        <v>271</v>
       </c>
       <c r="K5">
-        <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <f>33*33*3</f>
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C36" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D36" ca="1" si="1">RANDBETWEEN(100,500)</f>
-        <v>301</v>
+        <v>344</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E36" ca="1" si="2">RANDBETWEEN(1,1000)</f>
-        <v>697</v>
+        <v>29</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F36" ca="1" si="3">RANDBETWEEN(1,50)</f>
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G36" ca="1" si="4">RAND()</f>
-        <v>0.78124481137699153</v>
+        <v>0.1415828844870709</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H36" ca="1" si="5">RANDBETWEEN(1,100)</f>
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I36" ca="1" si="6">RANDBETWEEN(100,500)</f>
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J36" ca="1" si="7">RANDBETWEEN(1,1000)</f>
-        <v>580</v>
+        <v>70</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K36" ca="1" si="8">RANDBETWEEN(1,50)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="1"/>
-        <v>395</v>
+        <v>344</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="2"/>
-        <v>345</v>
+        <v>729</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.83424756989159143</v>
+        <v>0.83012254844926647</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="5"/>
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="6"/>
-        <v>201</v>
+        <v>427</v>
       </c>
       <c r="J7">
-        <f t="shared" ca="1" si="7"/>
-        <v>117</v>
+        <v>279</v>
       </c>
       <c r="K7">
-        <f t="shared" ca="1" si="8"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="1"/>
-        <v>287</v>
+        <v>364</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="2"/>
-        <v>295</v>
+        <v>1000</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.70011411001172297</v>
+        <v>0.46185387184344373</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="I8">
-        <f t="shared" ca="1" si="6"/>
-        <v>201</v>
+        <v>125</v>
       </c>
       <c r="J8">
-        <f t="shared" ca="1" si="7"/>
-        <v>274</v>
+        <v>509</v>
       </c>
       <c r="K8">
-        <f t="shared" ca="1" si="8"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>350</v>
+        <v>453</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="2"/>
-        <v>311</v>
+        <v>347</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48452393133716165</v>
+        <v>0.15248399193785789</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="5"/>
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="I9">
-        <f t="shared" ca="1" si="6"/>
-        <v>288</v>
+        <v>177</v>
       </c>
       <c r="J9">
-        <f t="shared" ca="1" si="7"/>
-        <v>598</v>
+        <v>527</v>
       </c>
       <c r="K9">
-        <f t="shared" ca="1" si="8"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="1"/>
-        <v>325</v>
+        <v>174</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="2"/>
-        <v>873</v>
+        <v>321</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.66232257435370701</v>
+        <v>0.33229817559609665</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="5"/>
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="I10">
-        <f t="shared" ca="1" si="6"/>
-        <v>431</v>
+        <v>482</v>
       </c>
       <c r="J10">
-        <f t="shared" ca="1" si="7"/>
-        <v>752</v>
+        <v>110</v>
       </c>
       <c r="K10">
-        <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="1"/>
-        <v>375</v>
+        <v>497</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="2"/>
-        <v>535</v>
+        <v>886</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.17492483484724786</v>
+        <v>0.237576126660344</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="5"/>
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="I11">
-        <f t="shared" ca="1" si="6"/>
-        <v>224</v>
+        <v>444</v>
       </c>
       <c r="J11">
-        <f t="shared" ca="1" si="7"/>
-        <v>32</v>
+        <v>648</v>
       </c>
       <c r="K11">
-        <f t="shared" ca="1" si="8"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="1"/>
-        <v>475</v>
+        <v>424</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="2"/>
-        <v>853</v>
+        <v>817</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.23191537805853291</v>
+        <v>0.66803560014336527</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="5"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I12">
-        <f t="shared" ca="1" si="6"/>
-        <v>273</v>
+        <v>158</v>
       </c>
       <c r="J12">
-        <f t="shared" ca="1" si="7"/>
-        <v>652</v>
+        <v>712</v>
       </c>
       <c r="K12">
-        <f t="shared" ca="1" si="8"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="1"/>
-        <v>126</v>
+        <v>238</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="2"/>
-        <v>271</v>
+        <v>454</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.72881800762123494</v>
+        <v>0.73158928407732504</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="5"/>
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="I13">
-        <f t="shared" ca="1" si="6"/>
-        <v>184</v>
+        <v>252</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="7"/>
-        <v>744</v>
+        <v>83</v>
       </c>
       <c r="K13">
-        <f t="shared" ca="1" si="8"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="1"/>
+        <v>321</v>
+      </c>
+      <c r="E14">
+        <v>97</v>
+      </c>
+      <c r="F14">
+        <v>25</v>
+      </c>
+      <c r="G14">
+        <v>0.65840897711735491</v>
+      </c>
+      <c r="H14">
+        <v>65</v>
+      </c>
+      <c r="I14">
         <v>249</v>
       </c>
-      <c r="E14">
-        <f t="shared" ca="1" si="2"/>
-        <v>952</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ca="1" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48405616689631814</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="5"/>
-        <v>89</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ca="1" si="6"/>
-        <v>225</v>
-      </c>
       <c r="J14">
-        <f t="shared" ca="1" si="7"/>
-        <v>466</v>
+        <v>985</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="8"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="1"/>
-        <v>428</v>
+        <v>299</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="2"/>
-        <v>767</v>
+        <v>892</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.40458291174593186</v>
+        <v>0.44218222025731801</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="I15">
-        <f t="shared" ca="1" si="6"/>
-        <v>463</v>
+        <v>333</v>
       </c>
       <c r="J15">
-        <f t="shared" ca="1" si="7"/>
-        <v>372</v>
+        <v>676</v>
       </c>
       <c r="K15">
-        <f t="shared" ca="1" si="8"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="1"/>
-        <v>464</v>
+        <v>100</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="2"/>
-        <v>955</v>
+        <v>672</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.11536025025368679</v>
+        <v>0.82949956100869349</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="5"/>
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="I16">
-        <f t="shared" ca="1" si="6"/>
-        <v>483</v>
+        <v>284</v>
       </c>
       <c r="J16">
-        <f t="shared" ca="1" si="7"/>
-        <v>28</v>
+        <v>760</v>
       </c>
       <c r="K16">
-        <f t="shared" ca="1" si="8"/>
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1670,40 +1586,31 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>355</v>
+        <v>199</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="2"/>
-        <v>521</v>
+        <v>678</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.98411997493609116</v>
+        <v>0.85858261970619731</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="5"/>
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="I17">
-        <f t="shared" ca="1" si="6"/>
-        <v>357</v>
+        <v>235</v>
       </c>
       <c r="J17">
-        <f t="shared" ca="1" si="7"/>
-        <v>427</v>
+        <v>146</v>
       </c>
       <c r="K17">
-        <f t="shared" ca="1" si="8"/>
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1711,40 +1618,31 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D18">
-        <f t="shared" ca="1" si="1"/>
-        <v>484</v>
+        <v>432</v>
       </c>
       <c r="E18">
-        <f t="shared" ca="1" si="2"/>
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.53833626561366477</v>
+        <v>0.1127987236570408</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="I18">
-        <f t="shared" ca="1" si="6"/>
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="J18">
-        <f t="shared" ca="1" si="7"/>
-        <v>666</v>
+        <v>722</v>
       </c>
       <c r="K18">
-        <f t="shared" ca="1" si="8"/>
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1752,40 +1650,31 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <f t="shared" ca="1" si="1"/>
-        <v>394</v>
+        <v>474</v>
       </c>
       <c r="E19">
-        <f t="shared" ca="1" si="2"/>
-        <v>976</v>
+        <v>811</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.58521165618830961</v>
+        <v>0.63259352546140257</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="I19">
-        <f t="shared" ca="1" si="6"/>
-        <v>381</v>
+        <v>220</v>
       </c>
       <c r="J19">
-        <f t="shared" ca="1" si="7"/>
-        <v>851</v>
+        <v>978</v>
       </c>
       <c r="K19">
-        <f t="shared" ca="1" si="8"/>
-        <v>47</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1793,40 +1682,31 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="D20">
-        <f t="shared" ca="1" si="1"/>
-        <v>448</v>
+        <v>124</v>
       </c>
       <c r="E20">
-        <f t="shared" ca="1" si="2"/>
-        <v>852</v>
+        <v>868</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.65863893009722863</v>
+        <v>0.42504126213914606</v>
       </c>
       <c r="H20">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="I20">
-        <f t="shared" ca="1" si="6"/>
-        <v>211</v>
+        <v>379</v>
       </c>
       <c r="J20">
-        <f t="shared" ca="1" si="7"/>
-        <v>634</v>
+        <v>787</v>
       </c>
       <c r="K20">
-        <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1834,40 +1714,31 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="0"/>
         <v>87</v>
       </c>
       <c r="D21">
-        <f t="shared" ca="1" si="1"/>
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="E21">
-        <f t="shared" ca="1" si="2"/>
-        <v>270</v>
+        <v>979</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.50422933616342491</v>
+        <v>0.73368924880898934</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I21">
-        <f t="shared" ca="1" si="6"/>
-        <v>500</v>
+        <v>446</v>
       </c>
       <c r="J21">
-        <f t="shared" ca="1" si="7"/>
-        <v>350</v>
+        <v>94</v>
       </c>
       <c r="K21">
-        <f t="shared" ca="1" si="8"/>
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1875,39 +1746,30 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D22">
-        <f t="shared" ca="1" si="1"/>
-        <v>257</v>
+        <v>310</v>
       </c>
       <c r="E22">
-        <f t="shared" ca="1" si="2"/>
-        <v>809</v>
+        <v>19</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.72110370819582725</v>
+        <v>0.51712433760296961</v>
       </c>
       <c r="H22">
-        <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I22">
-        <f t="shared" ca="1" si="6"/>
-        <v>285</v>
+        <v>362</v>
       </c>
       <c r="J22">
-        <f t="shared" ca="1" si="7"/>
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="K22">
-        <f t="shared" ca="1" si="8"/>
         <v>47</v>
       </c>
     </row>
@@ -1916,40 +1778,31 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="D23">
-        <f t="shared" ca="1" si="1"/>
-        <v>393</v>
+        <v>107</v>
       </c>
       <c r="E23">
-        <f t="shared" ca="1" si="2"/>
-        <v>333</v>
+        <v>977</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="G23">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.6522630815053239E-2</v>
+        <v>0.93896529830853936</v>
       </c>
       <c r="H23">
-        <f t="shared" ca="1" si="5"/>
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="I23">
-        <f t="shared" ca="1" si="6"/>
-        <v>386</v>
+        <v>260</v>
       </c>
       <c r="J23">
-        <f t="shared" ca="1" si="7"/>
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="K23">
-        <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1957,40 +1810,31 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D24">
-        <f t="shared" ca="1" si="1"/>
-        <v>107</v>
+        <v>427</v>
       </c>
       <c r="E24">
-        <f t="shared" ca="1" si="2"/>
-        <v>330</v>
+        <v>104</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.14138610637360283</v>
+        <v>0.10028367824032813</v>
       </c>
       <c r="H24">
-        <f t="shared" ca="1" si="5"/>
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I24">
-        <f t="shared" ca="1" si="6"/>
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="J24">
-        <f t="shared" ca="1" si="7"/>
-        <v>343</v>
+        <v>230</v>
       </c>
       <c r="K24">
-        <f t="shared" ca="1" si="8"/>
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1998,40 +1842,31 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D25">
-        <f t="shared" ca="1" si="1"/>
-        <v>421</v>
+        <v>358</v>
       </c>
       <c r="E25">
-        <f t="shared" ca="1" si="2"/>
-        <v>636</v>
+        <v>890</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G25">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.38403282323303523</v>
+        <v>0.96489106468780006</v>
       </c>
       <c r="H25">
-        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>400</v>
+      </c>
+      <c r="J25">
+        <v>426</v>
+      </c>
+      <c r="K25">
         <v>35</v>
-      </c>
-      <c r="I25">
-        <f t="shared" ca="1" si="6"/>
-        <v>352</v>
-      </c>
-      <c r="J25">
-        <f t="shared" ca="1" si="7"/>
-        <v>161</v>
-      </c>
-      <c r="K25">
-        <f t="shared" ca="1" si="8"/>
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -2039,40 +1874,31 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="D26">
-        <f t="shared" ca="1" si="1"/>
-        <v>352</v>
+        <v>424</v>
       </c>
       <c r="E26">
-        <f t="shared" ca="1" si="2"/>
-        <v>346</v>
+        <v>55</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G26">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.32033227604975467</v>
+        <v>0.41710079989282767</v>
       </c>
       <c r="H26">
-        <f t="shared" ca="1" si="5"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I26">
-        <f t="shared" ca="1" si="6"/>
-        <v>383</v>
+        <v>428</v>
       </c>
       <c r="J26">
-        <f t="shared" ca="1" si="7"/>
-        <v>610</v>
+        <v>419</v>
       </c>
       <c r="K26">
-        <f t="shared" ca="1" si="8"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -2080,40 +1906,31 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D27">
-        <f t="shared" ca="1" si="1"/>
-        <v>335</v>
+        <v>161</v>
       </c>
       <c r="E27">
-        <f t="shared" ca="1" si="2"/>
-        <v>150</v>
+        <v>206</v>
       </c>
       <c r="F27">
-        <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G27">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.46281272814794672</v>
+        <v>0.42375807787694497</v>
       </c>
       <c r="H27">
-        <f t="shared" ca="1" si="5"/>
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="I27">
-        <f t="shared" ca="1" si="6"/>
-        <v>491</v>
+        <v>176</v>
       </c>
       <c r="J27">
-        <f t="shared" ca="1" si="7"/>
-        <v>281</v>
+        <v>438</v>
       </c>
       <c r="K27">
-        <f t="shared" ca="1" si="8"/>
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -2121,40 +1938,31 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>306</v>
+      </c>
+      <c r="E28">
+        <v>651</v>
+      </c>
+      <c r="F28">
         <v>40</v>
       </c>
-      <c r="D28">
-        <f t="shared" ca="1" si="1"/>
-        <v>325</v>
-      </c>
-      <c r="E28">
-        <f t="shared" ca="1" si="2"/>
-        <v>362</v>
-      </c>
-      <c r="F28">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
       <c r="G28">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.61349740835547006</v>
+        <v>0.73394172028387639</v>
       </c>
       <c r="H28">
-        <f t="shared" ca="1" si="5"/>
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I28">
-        <f t="shared" ca="1" si="6"/>
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="J28">
-        <f t="shared" ca="1" si="7"/>
-        <v>376</v>
+        <v>147</v>
       </c>
       <c r="K28">
-        <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -2162,40 +1970,31 @@
         <v>47</v>
       </c>
       <c r="C29">
-        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D29">
+        <v>414</v>
+      </c>
+      <c r="E29">
+        <v>653</v>
+      </c>
+      <c r="F29">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <v>7.2717549899539269E-2</v>
+      </c>
+      <c r="H29">
         <v>22</v>
       </c>
-      <c r="D29">
-        <f t="shared" ca="1" si="1"/>
-        <v>268</v>
-      </c>
-      <c r="E29">
-        <f t="shared" ca="1" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="F29">
-        <f t="shared" ca="1" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="G29">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.52681639478576214</v>
-      </c>
-      <c r="H29">
-        <f t="shared" ca="1" si="5"/>
-        <v>24</v>
-      </c>
       <c r="I29">
-        <f t="shared" ca="1" si="6"/>
-        <v>355</v>
+        <v>274</v>
       </c>
       <c r="J29">
-        <f t="shared" ca="1" si="7"/>
-        <v>246</v>
+        <v>300</v>
       </c>
       <c r="K29">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -2203,40 +2002,31 @@
         <v>48</v>
       </c>
       <c r="C30">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="D30">
-        <f t="shared" ca="1" si="1"/>
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E30">
-        <f t="shared" ca="1" si="2"/>
-        <v>581</v>
+        <v>416</v>
       </c>
       <c r="F30">
-        <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G30">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.99787786997074357</v>
+        <v>0.56657876408655661</v>
       </c>
       <c r="H30">
-        <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="I30">
-        <f t="shared" ca="1" si="6"/>
-        <v>252</v>
+        <v>169</v>
       </c>
       <c r="J30">
-        <f t="shared" ca="1" si="7"/>
-        <v>841</v>
+        <v>403</v>
       </c>
       <c r="K30">
-        <f t="shared" ca="1" si="8"/>
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -2244,40 +2034,31 @@
         <v>49</v>
       </c>
       <c r="C31">
-        <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D31">
-        <f t="shared" ca="1" si="1"/>
-        <v>131</v>
+        <v>379</v>
       </c>
       <c r="E31">
-        <f t="shared" ca="1" si="2"/>
-        <v>232</v>
+        <v>820</v>
       </c>
       <c r="F31">
-        <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G31">
-        <f t="shared" ca="1" si="4"/>
-        <v>6.2524247115530729E-2</v>
+        <v>6.3529389039527095E-2</v>
       </c>
       <c r="H31">
-        <f t="shared" ca="1" si="5"/>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I31">
-        <f t="shared" ca="1" si="6"/>
-        <v>384</v>
+        <v>462</v>
       </c>
       <c r="J31">
-        <f t="shared" ca="1" si="7"/>
-        <v>834</v>
+        <v>758</v>
       </c>
       <c r="K31">
-        <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -2285,40 +2066,31 @@
         <v>50</v>
       </c>
       <c r="C32">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="D32">
-        <f t="shared" ca="1" si="1"/>
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E32">
-        <f t="shared" ca="1" si="2"/>
-        <v>379</v>
+        <v>574</v>
       </c>
       <c r="F32">
-        <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G32">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.6273079387500321</v>
+        <v>0.6927959652356267</v>
       </c>
       <c r="H32">
-        <f t="shared" ca="1" si="5"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I32">
-        <f t="shared" ca="1" si="6"/>
-        <v>430</v>
+        <v>472</v>
       </c>
       <c r="J32">
-        <f t="shared" ca="1" si="7"/>
-        <v>978</v>
+        <v>667</v>
       </c>
       <c r="K32">
-        <f t="shared" ca="1" si="8"/>
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
@@ -2326,40 +2098,31 @@
         <v>51</v>
       </c>
       <c r="C33">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="D33">
-        <f t="shared" ca="1" si="1"/>
-        <v>462</v>
+        <v>290</v>
       </c>
       <c r="E33">
-        <f t="shared" ca="1" si="2"/>
-        <v>660</v>
+        <v>230</v>
       </c>
       <c r="F33">
-        <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G33">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.14719800645779368</v>
+        <v>0.90936013445901787</v>
       </c>
       <c r="H33">
-        <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="I33">
-        <f t="shared" ca="1" si="6"/>
-        <v>424</v>
+        <v>368</v>
       </c>
       <c r="J33">
-        <f t="shared" ca="1" si="7"/>
-        <v>226</v>
+        <v>906</v>
       </c>
       <c r="K33">
-        <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
@@ -2367,40 +2130,31 @@
         <v>52</v>
       </c>
       <c r="C34">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D34">
-        <f t="shared" ca="1" si="1"/>
-        <v>456</v>
+        <v>382</v>
       </c>
       <c r="E34">
-        <f t="shared" ca="1" si="2"/>
-        <v>836</v>
+        <v>979</v>
       </c>
       <c r="F34">
-        <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G34">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.62326628847377219</v>
+        <v>0.98514101997312586</v>
       </c>
       <c r="H34">
-        <f t="shared" ca="1" si="5"/>
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="I34">
-        <f t="shared" ca="1" si="6"/>
-        <v>255</v>
+        <v>452</v>
       </c>
       <c r="J34">
-        <f t="shared" ca="1" si="7"/>
-        <v>755</v>
+        <v>312</v>
       </c>
       <c r="K34">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
@@ -2408,40 +2162,31 @@
         <v>53</v>
       </c>
       <c r="C35">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D35">
-        <f t="shared" ca="1" si="1"/>
-        <v>208</v>
+        <v>105</v>
       </c>
       <c r="E35">
-        <f t="shared" ca="1" si="2"/>
-        <v>178</v>
+        <v>858</v>
       </c>
       <c r="F35">
-        <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G35">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.59773812730504028</v>
+        <v>0.71497995154860339</v>
       </c>
       <c r="H35">
-        <f t="shared" ca="1" si="5"/>
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="I35">
-        <f t="shared" ca="1" si="6"/>
-        <v>290</v>
+        <v>454</v>
       </c>
       <c r="J35">
-        <f t="shared" ca="1" si="7"/>
-        <v>37</v>
+        <v>597</v>
       </c>
       <c r="K35">
-        <f t="shared" ca="1" si="8"/>
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -2449,40 +2194,31 @@
         <v>54</v>
       </c>
       <c r="C36">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="D36">
-        <f t="shared" ca="1" si="1"/>
         <v>386</v>
       </c>
       <c r="E36">
-        <f t="shared" ca="1" si="2"/>
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="G36">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.76419636186392526</v>
+        <v>0.34316074852813128</v>
       </c>
       <c r="H36">
-        <f t="shared" ca="1" si="5"/>
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="I36">
-        <f t="shared" ca="1" si="6"/>
-        <v>392</v>
+        <v>346</v>
       </c>
       <c r="J36">
-        <f t="shared" ca="1" si="7"/>
-        <v>256</v>
+        <v>308</v>
       </c>
       <c r="K36">
-        <f t="shared" ca="1" si="8"/>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -2528,48 +2264,48 @@
         <v>23</v>
       </c>
       <c r="C39">
-        <f ca="1">C5/SUM(C$5:C$36)</f>
-        <v>2.7745664739884393E-2</v>
+        <f>C5/SUM(C$5:C$36)</f>
+        <v>4.4080604534005039E-3</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:K39" ca="1" si="9">D5/SUM(D$5:D$36)</f>
-        <v>4.1654913023037143E-2</v>
+        <f t="shared" ref="D39:H39" si="0">D5/SUM(D$5:D$36)</f>
+        <v>3.3730765311321714E-2</v>
       </c>
       <c r="E39">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.0085480597749216E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.7585948778270867E-2</v>
       </c>
       <c r="F39">
-        <f t="array" aca="1" ref="F39" ca="1">(1/F5)/SUM(1/F$5:F$36)</f>
-        <v>2.7390956582732641E-2</v>
+        <f t="array" ref="F39">(1/F5)/SUM(1/F$5:F$36)</f>
+        <v>8.203918423897524E-3</v>
       </c>
       <c r="G39">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.614214001595041E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.7332475961059835E-3</v>
       </c>
       <c r="H39">
-        <f t="shared" ca="1" si="9"/>
-        <v>5.2516411378555797E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.2165775401069517E-2</v>
       </c>
       <c r="I39">
-        <f t="array" aca="1" ref="I39" ca="1">(1/I5)/SUM(1/I$5:I$36)</f>
-        <v>1.86238581680645E-2</v>
+        <f t="array" ref="I39">(1/I5)/SUM(1/I$5:I$36)</f>
+        <v>5.0345877346463196E-2</v>
       </c>
       <c r="J39">
-        <f t="array" aca="1" ref="J39" ca="1">(1/J5)/SUM(1/J$5:J$36)</f>
-        <v>3.1740682535092241E-2</v>
+        <f t="array" ref="J39">(1/J5)/SUM(1/J$5:J$36)</f>
+        <v>3.0384567960801429E-2</v>
       </c>
       <c r="K39">
-        <f t="array" aca="1" ref="K39" ca="1">(1/K5)/SUM(1/K$5:K$36)</f>
-        <v>8.5947425940880867E-3</v>
+        <f t="array" ref="K39">(1/K5)/SUM(1/K$5:K$36)</f>
+        <v>2.2105002840357112E-2</v>
       </c>
       <c r="M39">
-        <f ca="1">SUMPRODUCT(C39:K39,$C$77:$K$77)</f>
-        <v>2.3311974704697327E-2</v>
+        <f>SUMPRODUCT(C39:K39,$C$77:$K$77)</f>
+        <v>2.4860050272538046E-2</v>
       </c>
       <c r="N39">
-        <f ca="1">RANK(M39,$M$39:$M$70)</f>
-        <v>19</v>
+        <f>RANK(M39,$M$39:$M$70)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -2577,48 +2313,48 @@
         <v>24</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:K70" ca="1" si="10">C6/SUM(C$5:C$36)</f>
-        <v>3.7572254335260118E-2</v>
+        <f t="shared" ref="C40:H70" si="1">C6/SUM(C$5:C$36)</f>
+        <v>4.848866498740554E-2</v>
       </c>
       <c r="D40">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.8302773859896567E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.505553857128299E-2</v>
       </c>
       <c r="E40">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.2863292540434167E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5505533871571406E-3</v>
       </c>
       <c r="F40">
-        <f t="array" aca="1" ref="F40" ca="1">(1/F6)/SUM(1/F$5:F$36)</f>
-        <v>2.9102891369153432E-2</v>
+        <f t="array" ref="F40">(1/F6)/SUM(1/F$5:F$36)</f>
+        <v>3.7738024749928607E-3</v>
       </c>
       <c r="G40">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.837442815911995E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.4500768811436415E-3</v>
       </c>
       <c r="H40">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.4070021881838075E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.9465240641711233E-2</v>
       </c>
       <c r="I40">
-        <f t="array" aca="1" ref="I40" ca="1">(1/I6)/SUM(1/I$5:I$36)</f>
-        <v>2.7421631658499881E-2</v>
+        <f t="array" ref="I40">(1/I6)/SUM(1/I$5:I$36)</f>
+        <v>2.4201875757053525E-2</v>
       </c>
       <c r="J40">
-        <f t="array" aca="1" ref="J40" ca="1">(1/J6)/SUM(1/J$5:J$36)</f>
-        <v>9.7411060193903793E-3</v>
+        <f t="array" ref="J40">(1/J6)/SUM(1/J$5:J$36)</f>
+        <v>0.11763168453395982</v>
       </c>
       <c r="K40">
-        <f t="array" aca="1" ref="K40" ca="1">(1/K6)/SUM(1/K$5:K$36)</f>
-        <v>7.6804082755680776E-3</v>
+        <f t="array" ref="K40">(1/K6)/SUM(1/K$5:K$36)</f>
+        <v>3.3683813851972742E-2</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40:M70" ca="1" si="11">SUMPRODUCT(C40:K40,$C$77:$K$77)</f>
-        <v>2.2192931582242906E-2</v>
+        <f t="shared" ref="M40:M70" si="2">SUMPRODUCT(C40:K40,$C$77:$K$77)</f>
+        <v>3.4946350756403947E-2</v>
       </c>
       <c r="N40">
-        <f t="shared" ref="N40:N70" ca="1" si="12">RANK(M40,$M$39:$M$70)</f>
-        <v>22</v>
+        <f t="shared" ref="N40:N70" si="3">RANK(M40,$M$39:$M$70)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -2626,48 +2362,48 @@
         <v>25</v>
       </c>
       <c r="C41">
-        <f t="shared" ca="1" si="10"/>
-        <v>8.0924855491329474E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.7229219143576827E-2</v>
       </c>
       <c r="D41">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.7141513869299481E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.505553857128299E-2</v>
       </c>
       <c r="E41">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.1216407355021217E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.8977704111639845E-2</v>
       </c>
       <c r="F41">
-        <f t="array" aca="1" ref="F41" ca="1">(1/F7)/SUM(1/F$5:F$36)</f>
-        <v>2.0245489648106737E-2</v>
+        <f t="array" ref="F41">(1/F7)/SUM(1/F$5:F$36)</f>
+        <v>0.18869012374964303</v>
       </c>
       <c r="G41">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.1656341967264839E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.9544119549335429E-2</v>
       </c>
       <c r="H41">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.1575492341356671E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.550802139037433E-2</v>
       </c>
       <c r="I41">
-        <f t="array" aca="1" ref="I41" ca="1">(1/I7)/SUM(1/I$5:I$36)</f>
-        <v>4.4474885177467463E-2</v>
+        <f t="array" ref="I41">(1/I7)/SUM(1/I$5:I$36)</f>
+        <v>1.9100777822311562E-2</v>
       </c>
       <c r="J41">
-        <f t="array" aca="1" ref="J41" ca="1">(1/J7)/SUM(1/J$5:J$36)</f>
-        <v>4.8289243514926666E-2</v>
+        <f t="array" ref="J41">(1/J7)/SUM(1/J$5:J$36)</f>
+        <v>2.9513325868735441E-2</v>
       </c>
       <c r="K41">
-        <f t="array" aca="1" ref="K41" ca="1">(1/K7)/SUM(1/K$5:K$36)</f>
-        <v>1.4439167558067987E-2</v>
+        <f t="array" ref="K41">(1/K7)/SUM(1/K$5:K$36)</f>
+        <v>2.4391727272118191E-2</v>
       </c>
       <c r="M41">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.8857153426484535E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.8327319277613411E-2</v>
       </c>
       <c r="N41">
-        <f t="shared" ca="1" si="12"/>
-        <v>11</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -2675,48 +2411,48 @@
         <v>26</v>
       </c>
       <c r="C42">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.4913294797687862E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.4080604534005039E-3</v>
       </c>
       <c r="D42">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.698636577338975E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.7093651278915722E-2</v>
       </c>
       <c r="E42">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.8141565709365967E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.3467358177832436E-2</v>
       </c>
       <c r="F42">
-        <f t="array" aca="1" ref="F42" ca="1">(1/F8)/SUM(1/F$5:F$36)</f>
-        <v>1.5521542063548497E-2</v>
+        <f t="array" ref="F42">(1/F8)/SUM(1/F$5:F$36)</f>
+        <v>4.1931138611031784E-3</v>
       </c>
       <c r="G42">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.3350841150873759E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.7564777614679476E-2</v>
       </c>
       <c r="H42">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.7505470459518599E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.7433155080213901E-2</v>
       </c>
       <c r="I42">
-        <f t="array" aca="1" ref="I42" ca="1">(1/I8)/SUM(1/I$5:I$36)</f>
-        <v>4.4474885177467463E-2</v>
+        <f t="array" ref="I42">(1/I8)/SUM(1/I$5:I$36)</f>
+        <v>6.5248257041016305E-2</v>
       </c>
       <c r="J42">
-        <f t="array" aca="1" ref="J42" ca="1">(1/J8)/SUM(1/J$5:J$36)</f>
-        <v>2.061985945710372E-2</v>
+        <f t="array" ref="J42">(1/J8)/SUM(1/J$5:J$36)</f>
+        <v>1.6177245417243982E-2</v>
       </c>
       <c r="K42">
-        <f t="array" aca="1" ref="K42" ca="1">(1/K8)/SUM(1/K$5:K$36)</f>
-        <v>1.0938763301566658E-2</v>
+        <f t="array" ref="K42">(1/K8)/SUM(1/K$5:K$36)</f>
+        <v>1.4147201817828551E-2</v>
       </c>
       <c r="M42">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.2257465423803954E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2274157429819592E-2</v>
       </c>
       <c r="N42">
-        <f t="shared" ca="1" si="12"/>
-        <v>21</v>
+        <f t="shared" si="3"/>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -2724,48 +2460,48 @@
         <v>27</v>
       </c>
       <c r="C43">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.5086705202312137E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6372795969773299E-2</v>
       </c>
       <c r="D43">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.2910202162670425E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.6163252827881383E-2</v>
       </c>
       <c r="E43">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.9125515035975649E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.8553173287707853E-2</v>
       </c>
       <c r="F43">
-        <f t="array" aca="1" ref="F43" ca="1">(1/F9)/SUM(1/F$5:F$36)</f>
-        <v>1.369547829136632E-2</v>
+        <f t="array" ref="F43">(1/F9)/SUM(1/F$5:F$36)</f>
+        <v>9.4345061874821515E-2</v>
       </c>
       <c r="G43">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.0001566431567067E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.1006865673530623E-3</v>
       </c>
       <c r="H43">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.8840262582056896E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.0160427807486629E-3</v>
       </c>
       <c r="I43">
-        <f t="array" aca="1" ref="I43" ca="1">(1/I9)/SUM(1/I$5:I$36)</f>
-        <v>3.1039763613440834E-2</v>
+        <f t="array" ref="I43">(1/I9)/SUM(1/I$5:I$36)</f>
+        <v>4.6079277571339193E-2</v>
       </c>
       <c r="J43">
-        <f t="array" aca="1" ref="J43" ca="1">(1/J9)/SUM(1/J$5:J$36)</f>
-        <v>9.4478954703117388E-3</v>
+        <f t="array" ref="J43">(1/J9)/SUM(1/J$5:J$36)</f>
+        <v>1.5624701930506997E-2</v>
       </c>
       <c r="K43">
-        <f t="array" aca="1" ref="K43" ca="1">(1/K9)/SUM(1/K$5:K$36)</f>
-        <v>2.2561199309481229E-2</v>
+        <f t="array" ref="K43">(1/K9)/SUM(1/K$5:K$36)</f>
+        <v>2.8294403635657103E-2</v>
       </c>
       <c r="M43">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.2099063165060127E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.0442274073450274E-2</v>
       </c>
       <c r="N43">
-        <f t="shared" ca="1" si="12"/>
-        <v>23</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -2773,48 +2509,48 @@
         <v>28</v>
       </c>
       <c r="C44">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.722543352601156E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.2972292191435767E-4</v>
       </c>
       <c r="D44">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.0559473436765398E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.773158055640477E-2</v>
       </c>
       <c r="E44">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.3686735133140644E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.7163021975084212E-2</v>
       </c>
       <c r="F44">
-        <f t="array" aca="1" ref="F44" ca="1">(1/F10)/SUM(1/F$5:F$36)</f>
-        <v>1.0122744824053368E-2</v>
+        <f t="array" ref="F44">(1/F10)/SUM(1/F$5:F$36)</f>
+        <v>3.9310442447842301E-3</v>
       </c>
       <c r="G44">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.1010801383455274E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.983251818483189E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.2122538293216633E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.0213903743315516E-3</v>
       </c>
       <c r="I44">
-        <f t="array" aca="1" ref="I44" ca="1">(1/I10)/SUM(1/I$5:I$36)</f>
-        <v>2.0741187750976706E-2</v>
+        <f t="array" ref="I44">(1/I10)/SUM(1/I$5:I$36)</f>
+        <v>1.6921228485740743E-2</v>
       </c>
       <c r="J44">
-        <f t="array" aca="1" ref="J44" ca="1">(1/J10)/SUM(1/J$5:J$36)</f>
-        <v>7.5130870894234304E-3</v>
+        <f t="array" ref="J44">(1/J10)/SUM(1/J$5:J$36)</f>
+        <v>7.4856526521610789E-2</v>
       </c>
       <c r="K44">
-        <f t="array" aca="1" ref="K44" ca="1">(1/K10)/SUM(1/K$5:K$36)</f>
-        <v>0.36097918895169967</v>
+        <f t="array" ref="K44">(1/K10)/SUM(1/K$5:K$36)</f>
+        <v>1.6450234671893663E-2</v>
       </c>
       <c r="M44">
-        <f t="shared" ca="1" si="11"/>
-        <v>0.11097943188169634</v>
+        <f t="shared" si="2"/>
+        <v>1.9384519838421595E-2</v>
       </c>
       <c r="N44">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
@@ -2822,48 +2558,48 @@
         <v>29</v>
       </c>
       <c r="C45">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.6994219653179193E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.2594458438287154E-2</v>
       </c>
       <c r="D45">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.5260930888575459E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.0647100784673389E-2</v>
       </c>
       <c r="E45">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.2900805608511163E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7372079345559537E-2</v>
       </c>
       <c r="F45">
-        <f t="array" aca="1" ref="F45" ca="1">(1/F11)/SUM(1/F$5:F$36)</f>
-        <v>1.5020847158272739E-2</v>
+        <f t="array" ref="F45">(1/F11)/SUM(1/F$5:F$36)</f>
+        <v>0.18869012374964303</v>
       </c>
       <c r="G45">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.0831289671734932E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4179231781278979E-2</v>
       </c>
       <c r="H45">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.3063457330415752E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.2112299465240643E-2</v>
       </c>
       <c r="I45">
-        <f t="array" aca="1" ref="I45" ca="1">(1/I11)/SUM(1/I$5:I$36)</f>
-        <v>3.9908267502995358E-2</v>
+        <f t="array" ref="I45">(1/I11)/SUM(1/I$5:I$36)</f>
+        <v>1.8369441734520355E-2</v>
       </c>
       <c r="J45">
-        <f t="array" aca="1" ref="J45" ca="1">(1/J11)/SUM(1/J$5:J$36)</f>
-        <v>0.17655754660145062</v>
+        <f t="array" ref="J45">(1/J11)/SUM(1/J$5:J$36)</f>
+        <v>1.2707126415705535E-2</v>
       </c>
       <c r="K45">
-        <f t="array" aca="1" ref="K45" ca="1">(1/K11)/SUM(1/K$5:K$36)</f>
-        <v>8.2040724761749933E-3</v>
+        <f t="array" ref="K45">(1/K11)/SUM(1/K$5:K$36)</f>
+        <v>2.8294403635657103E-2</v>
       </c>
       <c r="M45">
-        <f t="shared" ca="1" si="11"/>
-        <v>5.253157417797169E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.9399440924809097E-2</v>
       </c>
       <c r="N45">
-        <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
@@ -2871,48 +2607,48 @@
         <v>30</v>
       </c>
       <c r="C46">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.797687861271676E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.4634760705289674E-2</v>
       </c>
       <c r="D46">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.4663845792195581E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3207989401813918E-2</v>
       </c>
       <c r="E46">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.2456798474878545E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3682831631289096E-2</v>
       </c>
       <c r="F46">
-        <f t="array" aca="1" ref="F46" ca="1">(1/F12)/SUM(1/F$5:F$36)</f>
-        <v>1.5521542063548497E-2</v>
+        <f t="array" ref="F46">(1/F12)/SUM(1/F$5:F$36)</f>
+        <v>8.5768238068019559E-3</v>
       </c>
       <c r="G46">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.4360125829333666E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.9870300714687418E-2</v>
       </c>
       <c r="H46">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.6411378555798686E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0721925133689839E-2</v>
       </c>
       <c r="I46">
-        <f t="array" aca="1" ref="I46" ca="1">(1/I12)/SUM(1/I$5:I$36)</f>
-        <v>3.2745245130662862E-2</v>
+        <f t="array" ref="I46">(1/I12)/SUM(1/I$5:I$36)</f>
+        <v>5.1620456519791379E-2</v>
       </c>
       <c r="J46">
-        <f t="array" aca="1" ref="J46" ca="1">(1/J12)/SUM(1/J$5:J$36)</f>
-        <v>8.6654010601938947E-3</v>
+        <f t="array" ref="J46">(1/J12)/SUM(1/J$5:J$36)</f>
+        <v>1.1564912805305038E-2</v>
       </c>
       <c r="K46">
-        <f t="array" aca="1" ref="K46" ca="1">(1/K12)/SUM(1/K$5:K$36)</f>
-        <v>6.0163198158616607E-2</v>
+        <f t="array" ref="K46">(1/K12)/SUM(1/K$5:K$36)</f>
+        <v>3.5368004544571383E-2</v>
       </c>
       <c r="M46">
-        <f t="shared" ca="1" si="11"/>
-        <v>3.2537649772406287E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.6111974482892229E-2</v>
       </c>
       <c r="N46">
-        <f t="shared" ca="1" si="12"/>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -2920,47 +2656,47 @@
         <v>31</v>
       </c>
       <c r="C47">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.236994219653179E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6372795969773299E-2</v>
       </c>
       <c r="D47">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.1847672778561354E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.4253541220829511E-2</v>
       </c>
       <c r="E47">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.6665641719451448E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.4274180612735924E-2</v>
       </c>
       <c r="F47">
-        <f t="array" aca="1" ref="F47" ca="1">(1/F13)/SUM(1/F$5:F$36)</f>
-        <v>3.5818943223573457E-2</v>
+        <f t="array" ref="F47">(1/F13)/SUM(1/F$5:F$36)</f>
+        <v>1.1793132734352689E-2</v>
       </c>
       <c r="G47">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.5128177284922057E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3663368762901285E-2</v>
       </c>
       <c r="H47">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.2275711159737416E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="I47">
-        <f t="array" aca="1" ref="I47" ca="1">(1/I13)/SUM(1/I$5:I$36)</f>
-        <v>4.8583977829733484E-2</v>
+        <f t="array" ref="I47">(1/I13)/SUM(1/I$5:I$36)</f>
+        <v>3.236520686558348E-2</v>
       </c>
       <c r="J47">
-        <f t="array" aca="1" ref="J47" ca="1">(1/J13)/SUM(1/J$5:J$36)</f>
-        <v>7.5938729721054029E-3</v>
+        <f t="array" ref="J47">(1/J13)/SUM(1/J$5:J$36)</f>
+        <v>9.9207444787676971E-2</v>
       </c>
       <c r="K47">
-        <f t="array" aca="1" ref="K47" ca="1">(1/K13)/SUM(1/K$5:K$36)</f>
-        <v>6.0163198158616607E-2</v>
+        <f t="array" ref="K47">(1/K13)/SUM(1/K$5:K$36)</f>
+        <v>4.7157339392761836E-2</v>
       </c>
       <c r="M47">
-        <f t="shared" ca="1" si="11"/>
-        <v>3.4806448817439453E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.4117826942141549E-2</v>
       </c>
       <c r="N47">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
@@ -2969,48 +2705,48 @@
         <v>32</v>
       </c>
       <c r="C48">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.8728323699421967E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.4458438287153661E-3</v>
       </c>
       <c r="D48">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.3413258110014105E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2711708957505352E-2</v>
       </c>
       <c r="E48">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.8544984933275937E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.186333743249746E-3</v>
       </c>
       <c r="F48">
-        <f t="array" aca="1" ref="F48" ca="1">(1/F14)/SUM(1/F$5:F$36)</f>
-        <v>1.6056767651946722E-2</v>
+        <f t="array" ref="F48">(1/F14)/SUM(1/F$5:F$36)</f>
+        <v>7.5476049499857215E-3</v>
       </c>
       <c r="G48">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.9972602607411754E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.9295755952654381E-2</v>
       </c>
       <c r="H48">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.8687089715536105E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3449197860962567E-2</v>
       </c>
       <c r="I48">
-        <f t="array" aca="1" ref="I48" ca="1">(1/I14)/SUM(1/I$5:I$36)</f>
-        <v>3.9730897425204269E-2</v>
+        <f t="array" ref="I48">(1/I14)/SUM(1/I$5:I$36)</f>
+        <v>3.2755149116976051E-2</v>
       </c>
       <c r="J48">
-        <f t="array" aca="1" ref="J48" ca="1">(1/J14)/SUM(1/J$5:J$36)</f>
-        <v>1.2124123371773432E-2</v>
+        <f t="array" ref="J48">(1/J14)/SUM(1/J$5:J$36)</f>
+        <v>8.3596120988600892E-3</v>
       </c>
       <c r="K48">
-        <f t="array" aca="1" ref="K48" ca="1">(1/K14)/SUM(1/K$5:K$36)</f>
-        <v>1.2032639631723322E-2</v>
+        <f t="array" ref="K48">(1/K14)/SUM(1/K$5:K$36)</f>
+        <v>0.10105144155591822</v>
       </c>
       <c r="M48">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.3345893122306303E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.7318156421109512E-2</v>
       </c>
       <c r="N48">
-        <f t="shared" ca="1" si="12"/>
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
@@ -3018,48 +2754,48 @@
         <v>33</v>
       </c>
       <c r="C49">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.7341040462427746E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.5113350125944584E-2</v>
       </c>
       <c r="D49">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.024447578749412E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0469784979109345E-2</v>
       </c>
       <c r="E49">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.7168070844351519E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7692883494626533E-2</v>
       </c>
       <c r="F49">
-        <f t="array" aca="1" ref="F49" ca="1">(1/F15)/SUM(1/F$5:F$36)</f>
-        <v>1.2934618386290413E-2</v>
+        <f t="array" ref="F49">(1/F15)/SUM(1/F$5:F$36)</f>
+        <v>1.572417697913692E-2</v>
       </c>
       <c r="G49">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.5051644137213849E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.6390716435716752E-2</v>
       </c>
       <c r="H49">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.0087527352297593E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.9465240641711233E-2</v>
       </c>
       <c r="I49">
-        <f t="array" aca="1" ref="I49" ca="1">(1/I15)/SUM(1/I$5:I$36)</f>
-        <v>1.9307671534926484E-2</v>
+        <f t="array" ref="I49">(1/I15)/SUM(1/I$5:I$36)</f>
+        <v>2.4492588979360474E-2</v>
       </c>
       <c r="J49">
-        <f t="array" aca="1" ref="J49" ca="1">(1/J15)/SUM(1/J$5:J$36)</f>
-        <v>1.5187745944210806E-2</v>
+        <f t="array" ref="J49">(1/J15)/SUM(1/J$5:J$36)</f>
+        <v>1.218079573576507E-2</v>
       </c>
       <c r="K49">
-        <f t="array" aca="1" ref="K49" ca="1">(1/K15)/SUM(1/K$5:K$36)</f>
-        <v>8.8043704622365777E-3</v>
+        <f t="array" ref="K49">(1/K15)/SUM(1/K$5:K$36)</f>
+        <v>1.443592022227403E-2</v>
       </c>
       <c r="M49">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.7279255421849594E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.3328028861119135E-2</v>
       </c>
       <c r="N49">
-        <f t="shared" ca="1" si="12"/>
-        <v>31</v>
+        <f t="shared" si="3"/>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
@@ -3067,48 +2803,48 @@
         <v>34</v>
       </c>
       <c r="C50">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.6242774566473986E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.4080604534005039E-3</v>
       </c>
       <c r="D50">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.3629525152797367E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.0190563538163661E-2</v>
       </c>
       <c r="E50">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.8729475432015253E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5930064695503396E-2</v>
       </c>
       <c r="F50">
-        <f t="array" aca="1" ref="F50" ca="1">(1/F16)/SUM(1/F$5:F$36)</f>
-        <v>9.9073672746054237E-3</v>
+        <f t="array" ref="F50">(1/F16)/SUM(1/F$5:F$36)</f>
+        <v>9.4345061874821518E-3</v>
       </c>
       <c r="G50">
-        <f t="shared" ca="1" si="10"/>
-        <v>7.1430696972938921E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.95069378533423E-2</v>
       </c>
       <c r="H50">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.665207877461707E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0721925133689839E-2</v>
       </c>
       <c r="I50">
-        <f t="array" aca="1" ref="I50" ca="1">(1/I16)/SUM(1/I$5:I$36)</f>
-        <v>1.8508182030374663E-2</v>
+        <f t="array" ref="I50">(1/I16)/SUM(1/I$5:I$36)</f>
+        <v>2.8718422993405063E-2</v>
       </c>
       <c r="J50">
-        <f t="array" aca="1" ref="J50" ca="1">(1/J16)/SUM(1/J$5:J$36)</f>
-        <v>0.20178005325880069</v>
+        <f t="array" ref="J50">(1/J16)/SUM(1/J$5:J$36)</f>
+        <v>1.0834497259706826E-2</v>
       </c>
       <c r="K50">
-        <f t="array" aca="1" ref="K50" ca="1">(1/K16)/SUM(1/K$5:K$36)</f>
-        <v>1.336959959080369E-2</v>
+        <f t="array" ref="K50">(1/K16)/SUM(1/K$5:K$36)</f>
+        <v>1.6450234671893663E-2</v>
       </c>
       <c r="M50">
-        <f t="shared" ca="1" si="11"/>
-        <v>5.8440098920828333E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.8001318120088768E-2</v>
       </c>
       <c r="N50">
-        <f t="shared" ca="1" si="12"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
@@ -3116,48 +2852,48 @@
         <v>35</v>
       </c>
       <c r="C51">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.722543352601156E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7858942065491183E-2</v>
       </c>
       <c r="D51">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.3380347907851431E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0279221440945683E-2</v>
       </c>
       <c r="E51">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.203984994772769E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.6250868844570391E-2</v>
       </c>
       <c r="F51">
-        <f t="array" aca="1" ref="F51" ca="1">(1/F17)/SUM(1/F$5:F$36)</f>
-        <v>2.1165739177566135E-2</v>
+        <f t="array" ref="F51">(1/F17)/SUM(1/F$5:F$36)</f>
+        <v>1.572417697913692E-2</v>
       </c>
       <c r="G51">
-        <f t="shared" ca="1" si="10"/>
-        <v>6.0936393220445167E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.1242699084814894E-2</v>
       </c>
       <c r="H51">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.5404814004376369E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.2058823529411766E-2</v>
       </c>
       <c r="I51">
-        <f t="array" aca="1" ref="I51" ca="1">(1/I17)/SUM(1/I$5:I$36)</f>
-        <v>2.5040481570506892E-2</v>
+        <f t="array" ref="I51">(1/I17)/SUM(1/I$5:I$36)</f>
+        <v>3.4706519702668248E-2</v>
       </c>
       <c r="J51">
-        <f t="array" aca="1" ref="J51" ca="1">(1/J17)/SUM(1/J$5:J$36)</f>
-        <v>1.323147890221644E-2</v>
+        <f t="array" ref="J51">(1/J17)/SUM(1/J$5:J$36)</f>
+        <v>5.6398752858747861E-2</v>
       </c>
       <c r="K51">
-        <f t="array" aca="1" ref="K51" ca="1">(1/K17)/SUM(1/K$5:K$36)</f>
-        <v>3.2816289904699973E-2</v>
+        <f t="array" ref="K51">(1/K17)/SUM(1/K$5:K$36)</f>
+        <v>2.8294403635657103E-2</v>
       </c>
       <c r="M51">
-        <f t="shared" ca="1" si="11"/>
-        <v>3.0792915839947924E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.2741682442994163E-2</v>
       </c>
       <c r="N51">
-        <f t="shared" ca="1" si="12"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
@@ -3165,48 +2901,48 @@
         <v>36</v>
       </c>
       <c r="C52">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.0057803468208091E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7858942065491183E-2</v>
       </c>
       <c r="D52">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.5510108133521389E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.4023234484867016E-2</v>
       </c>
       <c r="E52">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.6098640919992618E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.1224937175854141E-2</v>
       </c>
       <c r="F52">
-        <f t="array" aca="1" ref="F52" ca="1">(1/F18)/SUM(1/F$5:F$36)</f>
-        <v>1.0347694709032332E-2</v>
+        <f t="array" ref="F52">(1/F18)/SUM(1/F$5:F$36)</f>
+        <v>1.8869012374964304E-2</v>
       </c>
       <c r="G52">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.333360891124134E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.7321547406664932E-3</v>
       </c>
       <c r="H52">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.4223194748358862E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.8074866310160429E-2</v>
       </c>
       <c r="I52">
-        <f t="array" aca="1" ref="I52" ca="1">(1/I18)/SUM(1/I$5:I$36)</f>
-        <v>5.1973557678319536E-2</v>
+        <f t="array" ref="I52">(1/I18)/SUM(1/I$5:I$36)</f>
+        <v>4.531128961181688E-2</v>
       </c>
       <c r="J52">
-        <f t="array" aca="1" ref="J52" ca="1">(1/J18)/SUM(1/J$5:J$36)</f>
-        <v>8.4832454823519816E-3</v>
+        <f t="array" ref="J52">(1/J18)/SUM(1/J$5:J$36)</f>
+        <v>1.1404733957586132E-2</v>
       </c>
       <c r="K52">
-        <f t="array" aca="1" ref="K52" ca="1">(1/K18)/SUM(1/K$5:K$36)</f>
-        <v>8.2040724761749933E-3</v>
+        <f t="array" ref="K52">(1/K18)/SUM(1/K$5:K$36)</f>
+        <v>3.5368004544571383E-2</v>
       </c>
       <c r="M52">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.7941224191377923E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.6521765000244009E-2</v>
       </c>
       <c r="N52">
-        <f t="shared" ca="1" si="12"/>
-        <v>29</v>
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -3214,48 +2950,48 @@
         <v>37</v>
       </c>
       <c r="C53">
-        <f t="shared" ca="1" si="10"/>
-        <v>9.2485549132947983E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.4483627204030227E-2</v>
       </c>
       <c r="D53">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.7047484720263278E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.8303271170895751E-2</v>
       </c>
       <c r="E53">
-        <f t="shared" ca="1" si="10"/>
-        <v>6.0020908923190452E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.33620274822221E-2</v>
       </c>
       <c r="F53">
-        <f t="array" aca="1" ref="F53" ca="1">(1/F19)/SUM(1/F$5:F$36)</f>
-        <v>4.6564626190645497E-2</v>
+        <f t="array" ref="F53">(1/F19)/SUM(1/F$5:F$36)</f>
+        <v>3.9310442447842301E-3</v>
       </c>
       <c r="G53">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.6236118061717636E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.7755014979587366E-2</v>
       </c>
       <c r="H53">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.8687089715536105E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.537433155080214E-2</v>
       </c>
       <c r="I53">
-        <f t="array" aca="1" ref="I53" ca="1">(1/I19)/SUM(1/I$5:I$36)</f>
-        <v>2.3463128400711183E-2</v>
+        <f t="array" ref="I53">(1/I19)/SUM(1/I$5:I$36)</f>
+        <v>3.7072873318759261E-2</v>
       </c>
       <c r="J53">
-        <f t="array" aca="1" ref="J53" ca="1">(1/J19)/SUM(1/J$5:J$36)</f>
-        <v>6.6390616818406811E-3</v>
+        <f t="array" ref="J53">(1/J19)/SUM(1/J$5:J$36)</f>
+        <v>8.4194457232895595E-3</v>
       </c>
       <c r="K53">
-        <f t="array" aca="1" ref="K53" ca="1">(1/K19)/SUM(1/K$5:K$36)</f>
-        <v>7.6804082755680776E-3</v>
+        <f t="array" ref="K53">(1/K19)/SUM(1/K$5:K$36)</f>
+        <v>0.11789334848190458</v>
       </c>
       <c r="M53">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.4870435938132745E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.0304906950366261E-2</v>
       </c>
       <c r="N53">
-        <f t="shared" ca="1" si="12"/>
-        <v>16</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
@@ -3263,48 +2999,48 @@
         <v>38</v>
       </c>
       <c r="C54">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.5086705202312137E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.5743073047858942E-2</v>
       </c>
       <c r="D54">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.2125058768218149E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.2636298787322938E-2</v>
       </c>
       <c r="E54">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.2395301641965437E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.6409666898358549E-2</v>
       </c>
       <c r="F54">
-        <f t="array" aca="1" ref="F54" ca="1">(1/F20)/SUM(1/F$5:F$36)</f>
-        <v>0.15521542063548496</v>
+        <f t="array" ref="F54">(1/F20)/SUM(1/F$5:F$36)</f>
+        <v>5.7178825378679712E-3</v>
       </c>
       <c r="G54">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.0782711312514916E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.53676943773673E-2</v>
       </c>
       <c r="H54">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.8293216630196935E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.6818181818181816E-2</v>
       </c>
       <c r="I54">
-        <f t="array" aca="1" ref="I54" ca="1">(1/I20)/SUM(1/I$5:I$36)</f>
-        <v>4.2367070714080385E-2</v>
+        <f t="array" ref="I54">(1/I20)/SUM(1/I$5:I$36)</f>
+        <v>2.1519873694266591E-2</v>
       </c>
       <c r="J54">
-        <f t="array" aca="1" ref="J54" ca="1">(1/J20)/SUM(1/J$5:J$36)</f>
-        <v>8.9114219104833112E-3</v>
+        <f t="array" ref="J54">(1/J20)/SUM(1/J$5:J$36)</f>
+        <v>1.0462792779386516E-2</v>
       </c>
       <c r="K54">
-        <f t="array" aca="1" ref="K54" ca="1">(1/K20)/SUM(1/K$5:K$36)</f>
-        <v>1.3883814959680758E-2</v>
+        <f t="array" ref="K54">(1/K20)/SUM(1/K$5:K$36)</f>
+        <v>1.7252685143693356E-2</v>
       </c>
       <c r="M54">
-        <f t="shared" ca="1" si="11"/>
-        <v>4.7374381203207007E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.0103480875543023E-2</v>
       </c>
       <c r="N54">
-        <f t="shared" ca="1" si="12"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -3312,48 +3048,48 @@
         <v>39</v>
       </c>
       <c r="C55">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.0289017341040465E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.478589420654912E-2</v>
       </c>
       <c r="D55">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.4104372355430184E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6508712931825129E-2</v>
       </c>
       <c r="E55">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.6604144886538344E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2344543656097954E-2</v>
       </c>
       <c r="F55">
-        <f t="array" aca="1" ref="F55" ca="1">(1/F21)/SUM(1/F$5:F$36)</f>
-        <v>4.233147835513227E-2</v>
+        <f t="array" ref="F55">(1/F21)/SUM(1/F$5:F$36)</f>
+        <v>1.1099419044096649E-2</v>
       </c>
       <c r="G55">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.1221718778479051E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3788700744196482E-2</v>
       </c>
       <c r="H55">
-        <f t="shared" ca="1" si="10"/>
-        <v>6.0175054704595188E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="I55">
-        <f t="array" aca="1" ref="I55" ca="1">(1/I21)/SUM(1/I$5:I$36)</f>
-        <v>1.7878903841341921E-2</v>
+        <f t="array" ref="I55">(1/I21)/SUM(1/I$5:I$36)</f>
+        <v>1.8287067556338649E-2</v>
       </c>
       <c r="J55">
-        <f t="array" aca="1" ref="J55" ca="1">(1/J21)/SUM(1/J$5:J$36)</f>
-        <v>1.6142404260704055E-2</v>
+        <f t="array" ref="J55">(1/J21)/SUM(1/J$5:J$36)</f>
+        <v>8.7598062950821148E-2</v>
       </c>
       <c r="K55">
-        <f t="array" aca="1" ref="K55" ca="1">(1/K21)/SUM(1/K$5:K$36)</f>
-        <v>7.8473736728630356E-3</v>
+        <f t="array" ref="K55">(1/K21)/SUM(1/K$5:K$36)</f>
+        <v>4.4210005680714225E-2</v>
       </c>
       <c r="M55">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.1656895084625101E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.7001155989887312E-2</v>
       </c>
       <c r="N55">
-        <f t="shared" ca="1" si="12"/>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
@@ -3361,48 +3097,48 @@
         <v>40</v>
       </c>
       <c r="C56">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.0635838150289016E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0151133501259445E-2</v>
       </c>
       <c r="D56">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.4165491302303714E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.1590746968307347E-2</v>
       </c>
       <c r="E56">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.9750937826701924E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.0158798053788163E-3</v>
       </c>
       <c r="F56">
-        <f t="array" aca="1" ref="F56" ca="1">(1/F22)/SUM(1/F$5:F$36)</f>
-        <v>1.0122744824053368E-2</v>
+        <f t="array" ref="F56">(1/F22)/SUM(1/F$5:F$36)</f>
+        <v>7.8620884895684601E-3</v>
       </c>
       <c r="G56">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.4650510338635936E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0863479195853014E-2</v>
       </c>
       <c r="H56">
-        <f t="shared" ca="1" si="10"/>
-        <v>8.2056892778993428E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.06951871657754E-2</v>
       </c>
       <c r="I56">
-        <f t="array" aca="1" ref="I56" ca="1">(1/I22)/SUM(1/I$5:I$36)</f>
-        <v>3.1366497967266531E-2</v>
+        <f t="array" ref="I56">(1/I22)/SUM(1/I$5:I$36)</f>
+        <v>2.2530475497588499E-2</v>
       </c>
       <c r="J56">
-        <f t="array" aca="1" ref="J56" ca="1">(1/J22)/SUM(1/J$5:J$36)</f>
-        <v>2.0323170831821655E-2</v>
+        <f t="array" ref="J56">(1/J22)/SUM(1/J$5:J$36)</f>
+        <v>2.5651769213013046E-2</v>
       </c>
       <c r="K56">
-        <f t="array" aca="1" ref="K56" ca="1">(1/K22)/SUM(1/K$5:K$36)</f>
-        <v>7.6804082755680776E-3</v>
+        <f t="array" ref="K56">(1/K22)/SUM(1/K$5:K$36)</f>
+        <v>1.5050214699817608E-2</v>
       </c>
       <c r="M56">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.9578231057932178E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.6304600910294981E-2</v>
       </c>
       <c r="N56">
-        <f t="shared" ca="1" si="12"/>
-        <v>26</v>
+        <f t="shared" si="3"/>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -3410,48 +3146,48 @@
         <v>41</v>
       </c>
       <c r="C57">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.4335260115606937E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.3299748110831235E-2</v>
       </c>
       <c r="D57">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.6953455571227083E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.0903902985835117E-2</v>
       </c>
       <c r="E57">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.0478445360063956E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2237608939742289E-2</v>
       </c>
       <c r="F57">
-        <f t="array" aca="1" ref="F57" ca="1">(1/F23)/SUM(1/F$5:F$36)</f>
-        <v>1.7909471611786729E-2</v>
+        <f t="array" ref="F57">(1/F23)/SUM(1/F$5:F$36)</f>
+        <v>4.8382083012728982E-3</v>
       </c>
       <c r="G57">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.6422727937127136E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.6040170308563536E-2</v>
       </c>
       <c r="H57">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.7592997811816196E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.0160427807486629E-3</v>
       </c>
       <c r="I57">
-        <f t="array" aca="1" ref="I57" ca="1">(1/I23)/SUM(1/I$5:I$36)</f>
-        <v>2.3159201867023214E-2</v>
+        <f t="array" ref="I57">(1/I23)/SUM(1/I$5:I$36)</f>
+        <v>3.1369354346642453E-2</v>
       </c>
       <c r="J57">
-        <f t="array" aca="1" ref="J57" ca="1">(1/J23)/SUM(1/J$5:J$36)</f>
-        <v>3.1563360286292849E-2</v>
+        <f t="array" ref="J57">(1/J23)/SUM(1/J$5:J$36)</f>
+        <v>6.4329827479509286E-2</v>
       </c>
       <c r="K57">
-        <f t="array" aca="1" ref="K57" ca="1">(1/K23)/SUM(1/K$5:K$36)</f>
-        <v>2.7767629919361516E-2</v>
+        <f t="array" ref="K57">(1/K23)/SUM(1/K$5:K$36)</f>
+        <v>1.911784029436291E-2</v>
       </c>
       <c r="M57">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.7850354804822237E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.7057541761956079E-2</v>
       </c>
       <c r="N57">
-        <f t="shared" ca="1" si="12"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -3459,48 +3195,48 @@
         <v>42</v>
       </c>
       <c r="C58">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.7745664739884393E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3853904282115869E-2</v>
       </c>
       <c r="D58">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.006111894687353E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3513706307958831E-2</v>
       </c>
       <c r="E58">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.0293954861324643E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.5606052504945727E-3</v>
       </c>
       <c r="F58">
-        <f t="array" aca="1" ref="F58" ca="1">(1/F24)/SUM(1/F$5:F$36)</f>
-        <v>3.5818943223573457E-2</v>
+        <f t="array" ref="F58">(1/F24)/SUM(1/F$5:F$36)</f>
+        <v>0.18869012374964303</v>
       </c>
       <c r="G58">
-        <f t="shared" ca="1" si="10"/>
-        <v>8.7545823612096129E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.9852205591420056E-3</v>
       </c>
       <c r="H58">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.3610503282275714E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.1497326203208559E-2</v>
       </c>
       <c r="I58">
-        <f t="array" aca="1" ref="I58" ca="1">(1/I24)/SUM(1/I$5:I$36)</f>
-        <v>6.0812598099802453E-2</v>
+        <f t="array" ref="I58">(1/I24)/SUM(1/I$5:I$36)</f>
+        <v>4.3383149628335303E-2</v>
       </c>
       <c r="J58">
-        <f t="array" aca="1" ref="J58" ca="1">(1/J24)/SUM(1/J$5:J$36)</f>
-        <v>1.6471841082351078E-2</v>
+        <f t="array" ref="J58">(1/J24)/SUM(1/J$5:J$36)</f>
+        <v>3.5800947466857337E-2</v>
       </c>
       <c r="K58">
-        <f t="array" aca="1" ref="K58" ca="1">(1/K24)/SUM(1/K$5:K$36)</f>
-        <v>8.394864859341853E-3</v>
+        <f t="array" ref="K58">(1/K24)/SUM(1/K$5:K$36)</f>
+        <v>4.1609417111260441E-2</v>
       </c>
       <c r="M58">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.2799206460448466E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.3064603825881216E-2</v>
       </c>
       <c r="N58">
-        <f t="shared" ca="1" si="12"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
@@ -3508,48 +3244,48 @@
         <v>43</v>
       </c>
       <c r="C59">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.4104046242774563E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.1007556675062973E-2</v>
       </c>
       <c r="D59">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.9586271744240717E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.6482217466625902E-2</v>
       </c>
       <c r="E59">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.9111985732734764E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7585948778270867E-2</v>
       </c>
       <c r="F59">
-        <f t="array" aca="1" ref="F59" ca="1">(1/F25)/SUM(1/F$5:F$36)</f>
-        <v>2.5869236772580826E-2</v>
+        <f t="array" ref="F59">(1/F25)/SUM(1/F$5:F$36)</f>
+        <v>1.7153647613603912E-2</v>
       </c>
       <c r="G59">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.3779189247333025E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.7587495184031286E-2</v>
       </c>
       <c r="H59">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.9146608315098467E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.6844919786096253E-4</v>
       </c>
       <c r="I59">
-        <f t="array" aca="1" ref="I59" ca="1">(1/I25)/SUM(1/I$5:I$36)</f>
-        <v>2.5396170229178866E-2</v>
+        <f t="array" ref="I59">(1/I25)/SUM(1/I$5:I$36)</f>
+        <v>2.0390080325317594E-2</v>
       </c>
       <c r="J59">
-        <f t="array" aca="1" ref="J59" ca="1">(1/J25)/SUM(1/J$5:J$36)</f>
-        <v>3.5092183175443596E-2</v>
+        <f t="array" ref="J59">(1/J25)/SUM(1/J$5:J$36)</f>
+        <v>1.9329150040791519E-2</v>
       </c>
       <c r="K59">
-        <f t="array" aca="1" ref="K59" ca="1">(1/K25)/SUM(1/K$5:K$36)</f>
-        <v>1.8998904681668403E-2</v>
+        <f t="array" ref="K59">(1/K25)/SUM(1/K$5:K$36)</f>
+        <v>2.0210288311183645E-2</v>
       </c>
       <c r="M59">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.7470438120115379E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.6811865969994183E-2</v>
       </c>
       <c r="N59">
-        <f t="shared" ca="1" si="12"/>
-        <v>13</v>
+        <f t="shared" si="3"/>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -3557,48 +3293,48 @@
         <v>44</v>
       </c>
       <c r="C60">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.6416184971098269E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.9823677581863979E-2</v>
       </c>
       <c r="D60">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.309826046074283E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3207989401813918E-2</v>
       </c>
       <c r="E60">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.1277904187934321E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.9407046997807838E-3</v>
       </c>
       <c r="F60">
-        <f t="array" aca="1" ref="F60" ca="1">(1/F26)/SUM(1/F$5:F$36)</f>
-        <v>1.2585034105579863E-2</v>
+        <f t="array" ref="F60">(1/F26)/SUM(1/F$5:F$36)</f>
+        <v>1.2579341583309535E-2</v>
       </c>
       <c r="G60">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.9834871795825163E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.4893784577490776E-2</v>
       </c>
       <c r="H60">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.2035010940919038E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3368983957219251E-2</v>
       </c>
       <c r="I60">
-        <f t="array" aca="1" ref="I60" ca="1">(1/I26)/SUM(1/I$5:I$36)</f>
-        <v>2.3340605536999896E-2</v>
+        <f t="array" ref="I60">(1/I26)/SUM(1/I$5:I$36)</f>
+        <v>1.9056149836745414E-2</v>
       </c>
       <c r="J60">
-        <f t="array" aca="1" ref="J60" ca="1">(1/J26)/SUM(1/J$5:J$36)</f>
-        <v>9.2620352315515072E-3</v>
+        <f t="array" ref="J60">(1/J26)/SUM(1/J$5:J$36)</f>
+        <v>1.9652071401854865E-2</v>
       </c>
       <c r="K60">
-        <f t="array" aca="1" ref="K60" ca="1">(1/K26)/SUM(1/K$5:K$36)</f>
-        <v>8.394864859341853E-3</v>
+        <f t="array" ref="K60">(1/K26)/SUM(1/K$5:K$36)</f>
+        <v>1.6841906925986371E-2</v>
       </c>
       <c r="M60">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.5022734236216024E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.1060654711745563E-2</v>
       </c>
       <c r="N60">
-        <f t="shared" ca="1" si="12"/>
-        <v>32</v>
+        <f t="shared" si="3"/>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -3606,48 +3342,48 @@
         <v>45</v>
       </c>
       <c r="C61">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.7803468208092483E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.6045340050377833E-2</v>
       </c>
       <c r="D61">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.1499764927127409E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6406807296443494E-2</v>
       </c>
       <c r="E61">
-        <f t="shared" ca="1" si="10"/>
-        <v>9.2245249369657459E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.1014275784633482E-2</v>
       </c>
       <c r="F61">
-        <f t="array" aca="1" ref="F61" ca="1">(1/F27)/SUM(1/F$5:F$36)</f>
-        <v>1.8625850476258199E-2</v>
+        <f t="array" ref="F61">(1/F27)/SUM(1/F$5:F$36)</f>
+        <v>4.2884119034009779E-3</v>
       </c>
       <c r="G61">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.8657215693322066E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.529111022167959E-2</v>
       </c>
       <c r="H61">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.1422319474835887E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.9465240641711233E-2</v>
       </c>
       <c r="I61">
-        <f t="array" aca="1" ref="I61" ca="1">(1/I27)/SUM(1/I$5:I$36)</f>
-        <v>1.8206623056356334E-2</v>
+        <f t="array" ref="I61">(1/I27)/SUM(1/I$5:I$36)</f>
+        <v>4.634109164844908E-2</v>
       </c>
       <c r="J61">
-        <f t="array" aca="1" ref="J61" ca="1">(1/J27)/SUM(1/J$5:J$36)</f>
-        <v>2.0106197477745263E-2</v>
+        <f t="array" ref="J61">(1/J27)/SUM(1/J$5:J$36)</f>
+        <v>1.8799584286249286E-2</v>
       </c>
       <c r="K61">
-        <f t="array" aca="1" ref="K61" ca="1">(1/K27)/SUM(1/K$5:K$36)</f>
-        <v>1.164448996618386E-2</v>
+        <f t="array" ref="K61">(1/K27)/SUM(1/K$5:K$36)</f>
+        <v>1.6076365702077898E-2</v>
       </c>
       <c r="M61">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.8822752693497272E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2743572064418953E-2</v>
       </c>
       <c r="N61">
-        <f t="shared" ca="1" si="12"/>
-        <v>28</v>
+        <f t="shared" si="3"/>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -3655,48 +3391,48 @@
         <v>46</v>
       </c>
       <c r="C62">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.3121387283236993E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.556675062972292E-3</v>
       </c>
       <c r="D62">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.0559473436765398E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.1183124426780801E-2</v>
       </c>
       <c r="E62">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.2261853514543999E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.4807250173768914E-2</v>
       </c>
       <c r="F62">
-        <f t="array" aca="1" ref="F62" ca="1">(1/F28)/SUM(1/F$5:F$36)</f>
-        <v>0.23282313095322746</v>
+        <f t="array" ref="F62">(1/F28)/SUM(1/F$5:F$36)</f>
+        <v>4.7172530937410759E-3</v>
       </c>
       <c r="G62">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.7987562764083396E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3803768973529569E-2</v>
       </c>
       <c r="H62">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.2122538293216633E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.7459893048128345E-2</v>
       </c>
       <c r="I62">
-        <f t="array" aca="1" ref="I62" ca="1">(1/I28)/SUM(1/I$5:I$36)</f>
-        <v>5.6939184208095295E-2</v>
+        <f t="array" ref="I62">(1/I28)/SUM(1/I$5:I$36)</f>
+        <v>5.510832520356107E-2</v>
       </c>
       <c r="J62">
-        <f t="array" aca="1" ref="J62" ca="1">(1/J28)/SUM(1/J$5:J$36)</f>
-        <v>1.5026174178846861E-2</v>
+        <f t="array" ref="J62">(1/J28)/SUM(1/J$5:J$36)</f>
+        <v>5.6015087873314197E-2</v>
       </c>
       <c r="K62">
-        <f t="array" aca="1" ref="K62" ca="1">(1/K28)/SUM(1/K$5:K$36)</f>
-        <v>2.4065279263446645E-2</v>
+        <f t="array" ref="K62">(1/K28)/SUM(1/K$5:K$36)</f>
+        <v>1.7684002272285691E-2</v>
       </c>
       <c r="M62">
-        <f t="shared" ca="1" si="11"/>
-        <v>6.413730757866036E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.8407248289988665E-2</v>
       </c>
       <c r="N62">
-        <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -3704,48 +3440,48 @@
         <v>47</v>
       </c>
       <c r="C63">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.2716763005780347E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5264483627204031E-2</v>
       </c>
       <c r="D63">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.5199811941701927E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.2188933047997555E-2</v>
       </c>
       <c r="E63">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.6604144886538342E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.4914184890124579E-2</v>
       </c>
       <c r="F63">
-        <f t="array" aca="1" ref="F63" ca="1">(1/F29)/SUM(1/F$5:F$36)</f>
-        <v>1.7909471611786729E-2</v>
+        <f t="array" ref="F63">(1/F29)/SUM(1/F$5:F$36)</f>
+        <v>7.2573124519093478E-3</v>
       </c>
       <c r="G63">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.2620302204238061E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3399941277197113E-3</v>
       </c>
       <c r="H63">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.3129102844638949E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="I63">
-        <f t="array" aca="1" ref="I63" ca="1">(1/I29)/SUM(1/I$5:I$36)</f>
-        <v>2.5181554706115383E-2</v>
+        <f t="array" ref="I63">(1/I29)/SUM(1/I$5:I$36)</f>
+        <v>2.9766540620901595E-2</v>
       </c>
       <c r="J63">
-        <f t="array" aca="1" ref="J63" ca="1">(1/J29)/SUM(1/J$5:J$36)</f>
-        <v>2.296683533027E-2</v>
+        <f t="array" ref="J63">(1/J29)/SUM(1/J$5:J$36)</f>
+        <v>2.7447393057923961E-2</v>
       </c>
       <c r="K63">
-        <f t="array" aca="1" ref="K63" ca="1">(1/K29)/SUM(1/K$5:K$36)</f>
-        <v>4.5122398618962459E-2</v>
+        <f t="array" ref="K63">(1/K29)/SUM(1/K$5:K$36)</f>
+        <v>2.0804708555630221E-2</v>
       </c>
       <c r="M63">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.5656239672944295E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.055096043285198E-2</v>
       </c>
       <c r="N63">
-        <f t="shared" ca="1" si="12"/>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
@@ -3753,48 +3489,48 @@
         <v>48</v>
       </c>
       <c r="C64">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.0982658959537572E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.4156171284634763E-2</v>
       </c>
       <c r="D64">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.7362482369534556E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.8941200448384795E-2</v>
       </c>
       <c r="E64">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.5729659922513993E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.2242421001978291E-2</v>
       </c>
       <c r="F64">
-        <f t="array" aca="1" ref="F64" ca="1">(1/F30)/SUM(1/F$5:F$36)</f>
-        <v>1.6630223639516245E-2</v>
+        <f t="array" ref="F64">(1/F30)/SUM(1/F$5:F$36)</f>
+        <v>7.2573124519093478E-3</v>
       </c>
       <c r="G64">
-        <f t="shared" ca="1" si="10"/>
-        <v>6.1788277668549808E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.3815062697016514E-2</v>
       </c>
       <c r="H64">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.1728665207877461E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.3475935828877004E-2</v>
       </c>
       <c r="I64">
-        <f t="array" aca="1" ref="I64" ca="1">(1/I30)/SUM(1/I$5:I$36)</f>
-        <v>3.5474015558218094E-2</v>
+        <f t="array" ref="I64">(1/I30)/SUM(1/I$5:I$36)</f>
+        <v>4.8260545148680695E-2</v>
       </c>
       <c r="J64">
-        <f t="array" aca="1" ref="J64" ca="1">(1/J30)/SUM(1/J$5:J$36)</f>
-        <v>6.7180041513037088E-3</v>
+        <f t="array" ref="J64">(1/J30)/SUM(1/J$5:J$36)</f>
+        <v>2.0432302524509151E-2</v>
       </c>
       <c r="K64">
-        <f t="array" aca="1" ref="K64" ca="1">(1/K30)/SUM(1/K$5:K$36)</f>
-        <v>9.0244797237924931E-3</v>
+        <f t="array" ref="K64">(1/K30)/SUM(1/K$5:K$36)</f>
+        <v>1.4147201817828551E-2</v>
       </c>
       <c r="M64">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.8950870203107071E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.627738997793775E-2</v>
       </c>
       <c r="N64">
-        <f t="shared" ca="1" si="12"/>
-        <v>27</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
@@ -3802,48 +3538,48 @@
         <v>49</v>
       </c>
       <c r="C65">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.4335260115606937E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.974811083123426E-2</v>
       </c>
       <c r="D65">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.231781852374236E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.8622235809640276E-2</v>
       </c>
       <c r="E65">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.4267265235840354E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3843233705822597E-2</v>
       </c>
       <c r="F65">
-        <f t="array" aca="1" ref="F65" ca="1">(1/F31)/SUM(1/F$5:F$36)</f>
-        <v>2.3282313095322749E-2</v>
+        <f t="array" ref="F65">(1/F31)/SUM(1/F$5:F$36)</f>
+        <v>3.7738024749928607E-2</v>
       </c>
       <c r="G65">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.8714813285765149E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.7916180585027591E-3</v>
       </c>
       <c r="H65">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.8599562363238512E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.0106951871657755E-2</v>
       </c>
       <c r="I65">
-        <f t="array" aca="1" ref="I65" ca="1">(1/I31)/SUM(1/I$5:I$36)</f>
-        <v>2.3279822710080625E-2</v>
+        <f t="array" ref="I65">(1/I31)/SUM(1/I$5:I$36)</f>
+        <v>1.7653749199409173E-2</v>
       </c>
       <c r="J65">
-        <f t="array" aca="1" ref="J65" ca="1">(1/J31)/SUM(1/J$5:J$36)</f>
-        <v>6.7743902772738843E-3</v>
+        <f t="array" ref="J65">(1/J31)/SUM(1/J$5:J$36)</f>
+        <v>1.0863084323716606E-2</v>
       </c>
       <c r="K65">
-        <f t="array" aca="1" ref="K65" ca="1">(1/K31)/SUM(1/K$5:K$36)</f>
-        <v>5.156845556452852E-2</v>
+        <f t="array" ref="K65">(1/K31)/SUM(1/K$5:K$36)</f>
+        <v>4.1609417111260441E-2</v>
       </c>
       <c r="M65">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.6788228291770133E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.2151753856793613E-2</v>
       </c>
       <c r="N65">
-        <f t="shared" ca="1" si="12"/>
-        <v>14</v>
+        <f t="shared" si="3"/>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
@@ -3851,48 +3587,48 @@
         <v>50</v>
       </c>
       <c r="C66">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.7803468208092489E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.2821158690176324E-2</v>
       </c>
       <c r="D66">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.8241654913023039E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0381127076327322E-2</v>
       </c>
       <c r="E66">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.3307299674066785E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0690263594075815E-2</v>
       </c>
       <c r="F66">
-        <f t="array" aca="1" ref="F66" ca="1">(1/F32)/SUM(1/F$5:F$36)</f>
-        <v>3.8803855158871241E-2</v>
+        <f t="array" ref="F66">(1/F32)/SUM(1/F$5:F$36)</f>
+        <v>6.2896707916547681E-2</v>
       </c>
       <c r="G66">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.8842706376792401E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.1348071063785657E-2</v>
       </c>
       <c r="H66">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.3129102844638949E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="I66">
-        <f t="array" aca="1" ref="I66" ca="1">(1/I32)/SUM(1/I$5:I$36)</f>
-        <v>2.0789423071327817E-2</v>
+        <f t="array" ref="I66">(1/I32)/SUM(1/I$5:I$36)</f>
+        <v>1.72797290892522E-2</v>
       </c>
       <c r="J66">
-        <f t="array" aca="1" ref="J66" ca="1">(1/J32)/SUM(1/J$5:J$36)</f>
-        <v>5.7769340401292637E-3</v>
+        <f t="array" ref="J66">(1/J32)/SUM(1/J$5:J$36)</f>
+        <v>1.2345154298916323E-2</v>
       </c>
       <c r="K66">
-        <f t="array" aca="1" ref="K66" ca="1">(1/K32)/SUM(1/K$5:K$36)</f>
-        <v>9.0244797237924931E-3</v>
+        <f t="array" ref="K66">(1/K32)/SUM(1/K$5:K$36)</f>
+        <v>2.5262860388979555E-2</v>
       </c>
       <c r="M66">
-        <f t="shared" ca="1" si="11"/>
-        <v>1.7389146213021071E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.5106996038532567E-2</v>
       </c>
       <c r="N66">
-        <f t="shared" ca="1" si="12"/>
-        <v>30</v>
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
@@ -3900,48 +3636,48 @@
         <v>51</v>
       </c>
       <c r="C67">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.6416184971098269E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.793450881612091E-2</v>
       </c>
       <c r="D67">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.3441466854724962E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.9552634260674615E-2</v>
       </c>
       <c r="E67">
-        <f t="shared" ca="1" si="10"/>
-        <v>4.0587909722649286E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.229749238090146E-2</v>
       </c>
       <c r="F67">
-        <f t="array" aca="1" ref="F67" ca="1">(1/F33)/SUM(1/F$5:F$36)</f>
-        <v>2.0245489648106737E-2</v>
+        <f t="array" ref="F67">(1/F33)/SUM(1/F$5:F$36)</f>
+        <v>7.8620884895684601E-3</v>
       </c>
       <c r="G67">
-        <f t="shared" ca="1" si="10"/>
-        <v>9.1144533504263405E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.427324832845544E-2</v>
       </c>
       <c r="H67">
-        <f t="shared" ca="1" si="10"/>
-        <v>3.5557986870897153E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.3475935828877002E-3</v>
       </c>
       <c r="I67">
-        <f t="array" aca="1" ref="I67" ca="1">(1/I33)/SUM(1/I$5:I$36)</f>
-        <v>2.1083613020450379E-2</v>
+        <f t="array" ref="I67">(1/I33)/SUM(1/I$5:I$36)</f>
+        <v>2.2163130788388687E-2</v>
       </c>
       <c r="J67">
-        <f t="array" aca="1" ref="J67" ca="1">(1/J33)/SUM(1/J$5:J$36)</f>
-        <v>2.4999298633833714E-2</v>
+        <f t="array" ref="J67">(1/J33)/SUM(1/J$5:J$36)</f>
+        <v>9.0885407476569407E-3</v>
       </c>
       <c r="K67">
-        <f t="array" aca="1" ref="K67" ca="1">(1/K33)/SUM(1/K$5:K$36)</f>
-        <v>1.5694747345726071E-2</v>
+        <f t="array" ref="K67">(1/K33)/SUM(1/K$5:K$36)</f>
+        <v>3.5368004544571383E-2</v>
       </c>
       <c r="M67">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.390081661713565E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2175248441129454E-2</v>
       </c>
       <c r="N67">
-        <f t="shared" ca="1" si="12"/>
-        <v>17</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
@@ -3949,48 +3685,48 @@
         <v>52</v>
       </c>
       <c r="C68">
-        <f t="shared" ca="1" si="10"/>
-        <v>2.7167630057803469E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.478589420654912E-2</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:K70" ca="1" si="13">D34/SUM(D$5:D$36)</f>
-        <v>4.2877291960507755E-2</v>
+        <f t="shared" ref="D68:H70" si="4">D34/SUM(D$5:D$36)</f>
+        <v>3.8927952715785183E-2</v>
       </c>
       <c r="E68">
-        <f t="shared" ca="1" si="13"/>
-        <v>5.1411352315355756E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.2344543656097954E-2</v>
       </c>
       <c r="F68">
-        <f t="array" aca="1" ref="F68" ca="1">(1/F34)/SUM(1/F$5:F$36)</f>
-        <v>1.1939647741191151E-2</v>
+        <f t="array" ref="F68">(1/F34)/SUM(1/F$5:F$36)</f>
+        <v>9.9310591447180543E-3</v>
       </c>
       <c r="G68">
-        <f t="shared" ca="1" si="13"/>
-        <v>3.8592448687927092E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.879607120379976E-2</v>
       </c>
       <c r="H68">
-        <f t="shared" ca="1" si="13"/>
-        <v>2.3522975929978117E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.6764705882352942E-2</v>
       </c>
       <c r="I68">
-        <f t="array" aca="1" ref="I68" ca="1">(1/I34)/SUM(1/I$5:I$36)</f>
-        <v>3.5056674198709649E-2</v>
+        <f t="array" ref="I68">(1/I34)/SUM(1/I$5:I$36)</f>
+        <v>1.8044318871962471E-2</v>
       </c>
       <c r="J68">
-        <f t="array" aca="1" ref="J68" ca="1">(1/J34)/SUM(1/J$5:J$36)</f>
-        <v>7.483233763240291E-3</v>
+        <f t="array" ref="J68">(1/J34)/SUM(1/J$5:J$36)</f>
+        <v>2.6391724094157652E-2</v>
       </c>
       <c r="K68">
-        <f t="array" aca="1" ref="K68" ca="1">(1/K34)/SUM(1/K$5:K$36)</f>
-        <v>7.2195837790339945E-2</v>
+        <f t="array" ref="K68">(1/K34)/SUM(1/K$5:K$36)</f>
+        <v>4.1609417111260441E-2</v>
       </c>
       <c r="M68">
-        <f t="shared" ca="1" si="11"/>
-        <v>3.5215532679381184E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.2591444299957723E-2</v>
       </c>
       <c r="N68">
-        <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
@@ -3998,48 +3734,48 @@
         <v>53</v>
       </c>
       <c r="C69">
-        <f t="shared" ca="1" si="10"/>
-        <v>1.8497109826589597E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.7153652392947101E-2</v>
       </c>
       <c r="D69">
-        <f t="shared" ca="1" si="13"/>
-        <v>1.9558062999529856E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.0700091715071844E-2</v>
       </c>
       <c r="E69">
-        <f t="shared" ca="1" si="13"/>
-        <v>1.0946436258532685E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.587499331658023E-2</v>
       </c>
       <c r="F69">
-        <f t="array" aca="1" ref="F69" ca="1">(1/F35)/SUM(1/F$5:F$36)</f>
-        <v>1.0347694709032332E-2</v>
+        <f t="array" ref="F69">(1/F35)/SUM(1/F$5:F$36)</f>
+        <v>5.7178825378679712E-3</v>
       </c>
       <c r="G69">
-        <f t="shared" ca="1" si="13"/>
-        <v>3.7011753135767642E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.2672075660485406E-2</v>
       </c>
       <c r="H69">
-        <f t="shared" ca="1" si="13"/>
-        <v>4.7045951859956234E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.1443850267379678E-2</v>
       </c>
       <c r="I69">
-        <f t="array" aca="1" ref="I69" ca="1">(1/I35)/SUM(1/I$5:I$36)</f>
-        <v>3.0825696278175725E-2</v>
+        <f t="array" ref="I69">(1/I35)/SUM(1/I$5:I$36)</f>
+        <v>1.7964828480456031E-2</v>
       </c>
       <c r="J69">
-        <f t="array" aca="1" ref="J69" ca="1">(1/J35)/SUM(1/J$5:J$36)</f>
-        <v>0.15269841868233566</v>
+        <f t="array" ref="J69">(1/J35)/SUM(1/J$5:J$36)</f>
+        <v>1.3792659828102492E-2</v>
       </c>
       <c r="K69">
-        <f t="array" aca="1" ref="K69" ca="1">(1/K35)/SUM(1/K$5:K$36)</f>
-        <v>9.4994523408342014E-3</v>
+        <f t="array" ref="K69">(1/K35)/SUM(1/K$5:K$36)</f>
+        <v>1.6076365702077898E-2</v>
       </c>
       <c r="M69">
-        <f t="shared" ca="1" si="11"/>
-        <v>4.4597979103260722E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.209181495356248E-2</v>
       </c>
       <c r="N69">
-        <f t="shared" ca="1" si="12"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
@@ -4047,48 +3783,48 @@
         <v>54</v>
       </c>
       <c r="C70">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.7803468208092489E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.1561712846347604E-2</v>
       </c>
       <c r="D70">
-        <f t="shared" ca="1" si="13"/>
-        <v>3.6295251527973672E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.9335575257311732E-2</v>
       </c>
       <c r="E70">
-        <f t="shared" ca="1" si="13"/>
-        <v>1.0946436258532685E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.1602416724589637E-2</v>
       </c>
       <c r="F70">
-        <f t="array" aca="1" ref="F70" ca="1">(1/F36)/SUM(1/F$5:F$36)</f>
-        <v>1.0122744824053368E-2</v>
+        <f t="array" ref="F70">(1/F36)/SUM(1/F$5:F$36)</f>
+        <v>2.096556930551589E-2</v>
       </c>
       <c r="G70">
-        <f t="shared" ca="1" si="13"/>
-        <v>4.7318793633060692E-2</v>
+        <f t="shared" si="4"/>
+        <v>2.0480828019281579E-2</v>
       </c>
       <c r="H70">
-        <f t="shared" ca="1" si="13"/>
-        <v>3.1181619256017507E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.0802139037433157E-2</v>
       </c>
       <c r="I70">
-        <f t="array" aca="1" ref="I70" ca="1">(1/I36)/SUM(1/I$5:I$36)</f>
-        <v>2.2804724287425918E-2</v>
+        <f t="array" ref="I70">(1/I36)/SUM(1/I$5:I$36)</f>
+        <v>2.3572347196898952E-2</v>
       </c>
       <c r="J70">
-        <f t="array" aca="1" ref="J70" ca="1">(1/J36)/SUM(1/J$5:J$36)</f>
-        <v>2.2069693325181328E-2</v>
+        <f t="array" ref="J70">(1/J36)/SUM(1/J$5:J$36)</f>
+        <v>2.6734473757718143E-2</v>
       </c>
       <c r="K70">
-        <f t="array" aca="1" ref="K70" ca="1">(1/K36)/SUM(1/K$5:K$36)</f>
-        <v>2.2561199309481229E-2</v>
+        <f t="array" ref="K70">(1/K36)/SUM(1/K$5:K$36)</f>
+        <v>3.3683813851972742E-2</v>
       </c>
       <c r="M70">
-        <f t="shared" ca="1" si="11"/>
-        <v>2.0545369593610439E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.8419895805512858E-2</v>
       </c>
       <c r="N70">
-        <f t="shared" ca="1" si="12"/>
-        <v>25</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
@@ -4096,40 +3832,40 @@
         <v>66</v>
       </c>
       <c r="C73">
-        <f ca="1">AVERAGE(C39:C70)</f>
+        <f>AVERAGE(C39:C70)</f>
+        <v>3.1250000000000007E-2</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ref="D73:K73" si="5">AVERAGE(D39:D70)</f>
         <v>3.125E-2</v>
       </c>
-      <c r="D73">
-        <f t="shared" ref="D73:K73" ca="1" si="14">AVERAGE(D39:D70)</f>
+      <c r="E73">
+        <f t="shared" si="5"/>
         <v>3.1249999999999997E-2</v>
       </c>
-      <c r="E73">
-        <f t="shared" ca="1" si="14"/>
-        <v>3.1249999999999997E-2</v>
-      </c>
       <c r="F73">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" si="5"/>
+        <v>3.1250000000000007E-2</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="5"/>
         <v>3.1249999999999993E-2</v>
       </c>
-      <c r="G73">
-        <f t="shared" ca="1" si="14"/>
+      <c r="H73">
+        <f t="shared" si="5"/>
+        <v>3.1249999999999993E-2</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="5"/>
+        <v>3.1250000000000014E-2</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="5"/>
         <v>3.1250000000000007E-2</v>
       </c>
-      <c r="H73">
-        <f t="shared" ca="1" si="14"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="I73">
-        <f t="shared" ca="1" si="14"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="J73">
-        <f t="shared" ca="1" si="14"/>
+      <c r="K73">
+        <f t="shared" si="5"/>
         <v>3.1250000000000007E-2</v>
-      </c>
-      <c r="K73">
-        <f t="shared" ca="1" si="14"/>
-        <v>3.124999999999999E-2</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
@@ -4137,40 +3873,40 @@
         <v>14</v>
       </c>
       <c r="C74">
-        <f ca="1">STDEVA(C39:C70)</f>
-        <v>1.7838557348497357E-2</v>
+        <f>STDEVA(C39:C70)</f>
+        <v>1.9767068818005998E-2</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74:K74" ca="1" si="15">STDEVA(D39:D70)</f>
-        <v>1.0357056338727204E-2</v>
+        <f t="shared" ref="D74:K74" si="6">STDEVA(D39:D70)</f>
+        <v>1.1953015770474602E-2</v>
       </c>
       <c r="E74">
-        <f t="shared" ca="1" si="15"/>
-        <v>1.7328595876783936E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.751097115540725E-2</v>
       </c>
       <c r="F74">
-        <f t="shared" ca="1" si="15"/>
-        <v>4.4959642822510276E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.4670417258503488E-2</v>
       </c>
       <c r="G74">
-        <f t="shared" ca="1" si="15"/>
-        <v>1.6140500426753402E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.7711666112301273E-2</v>
       </c>
       <c r="H74">
-        <f t="shared" ca="1" si="15"/>
-        <v>1.5733113487241442E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.9916442846122644E-2</v>
       </c>
       <c r="I74">
-        <f t="shared" ca="1" si="15"/>
-        <v>1.2052610769604816E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.3603369325086063E-2</v>
       </c>
       <c r="J74">
-        <f t="shared" ca="1" si="15"/>
-        <v>4.9038820785169912E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.8727176953676461E-2</v>
       </c>
       <c r="K74">
-        <f t="shared" ca="1" si="15"/>
-        <v>6.2772966765742483E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.2981152236290537E-2</v>
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
@@ -4178,40 +3914,40 @@
         <v>67</v>
       </c>
       <c r="C75">
-        <f ca="1">C74/C73</f>
-        <v>0.57083383515191544</v>
+        <f>C74/C73</f>
+        <v>0.63254620217619184</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:K75" ca="1" si="16">D74/D73</f>
-        <v>0.33142580283927059</v>
+        <f t="shared" ref="D75:K75" si="7">D74/D73</f>
+        <v>0.38249650465518725</v>
       </c>
       <c r="E75">
-        <f t="shared" ca="1" si="16"/>
-        <v>0.55451506805708606</v>
+        <f t="shared" si="7"/>
+        <v>0.5603510769730321</v>
       </c>
       <c r="F75">
-        <f t="shared" ca="1" si="16"/>
-        <v>1.4387085703203291</v>
+        <f t="shared" si="7"/>
+        <v>1.7494533522721112</v>
       </c>
       <c r="G75">
-        <f t="shared" ca="1" si="16"/>
-        <v>0.51649601365610875</v>
+        <f t="shared" si="7"/>
+        <v>0.56677331559364086</v>
       </c>
       <c r="H75">
-        <f t="shared" ca="1" si="16"/>
-        <v>0.50345963159172613</v>
+        <f t="shared" si="7"/>
+        <v>0.63732617107592471</v>
       </c>
       <c r="I75">
-        <f t="shared" ca="1" si="16"/>
-        <v>0.3856835446273541</v>
+        <f t="shared" si="7"/>
+        <v>0.43530781840275384</v>
       </c>
       <c r="J75">
-        <f t="shared" ca="1" si="16"/>
-        <v>1.5692422651254367</v>
+        <f t="shared" si="7"/>
+        <v>0.91926966251764652</v>
       </c>
       <c r="K75">
-        <f t="shared" ca="1" si="16"/>
-        <v>2.0087349365037603</v>
+        <f t="shared" si="7"/>
+        <v>0.73539687156129707</v>
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
@@ -4219,40 +3955,40 @@
         <v>68</v>
       </c>
       <c r="C77">
-        <f ca="1">C75/SUM($C$75:$K$75)</f>
-        <v>7.244911972360106E-2</v>
+        <f>C75/SUM($C$75:$K$75)</f>
+        <v>9.5566362635780402E-2</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:K77" ca="1" si="17">D75/SUM($C$75:$K$75)</f>
-        <v>4.2063918062955674E-2</v>
+        <f t="shared" ref="D77:K77" si="8">D75/SUM($C$75:$K$75)</f>
+        <v>5.7788347388756052E-2</v>
       </c>
       <c r="E77">
-        <f t="shared" ca="1" si="17"/>
-        <v>7.037797355427805E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.4658976753193213E-2</v>
       </c>
       <c r="F77">
-        <f t="shared" ca="1" si="17"/>
-        <v>0.18259809254433731</v>
+        <f t="shared" si="8"/>
+        <v>0.26431095926657516</v>
       </c>
       <c r="G77">
-        <f t="shared" ca="1" si="17"/>
-        <v>6.5552669140881689E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.562926158430767E-2</v>
       </c>
       <c r="H77">
-        <f t="shared" ca="1" si="17"/>
-        <v>6.3898116893302132E-2</v>
+        <f t="shared" si="8"/>
+        <v>9.6288530027961478E-2</v>
       </c>
       <c r="I77">
-        <f t="shared" ca="1" si="17"/>
-        <v>4.8950205084976647E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.5767187738296429E-2</v>
       </c>
       <c r="J77">
-        <f t="shared" ca="1" si="17"/>
-        <v>0.19916517511816978</v>
+        <f t="shared" si="8"/>
+        <v>0.13888512432134159</v>
       </c>
       <c r="K77">
-        <f t="shared" ca="1" si="17"/>
-        <v>0.25494472987749767</v>
+        <f t="shared" si="8"/>
+        <v>0.11110525028378797</v>
       </c>
     </row>
   </sheetData>
@@ -4271,4 +4007,62 @@
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2643E3BC-CAAB-4BA7-8FD4-0705D4316CFB}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>